<commit_message>
Update the similarity ratio between non-updated and updated summaries
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FCC3E8A-EECB-B34A-882B-D5A0A10EA706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BADCBA-D735-5245-9012-4478AA5AF37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="87">
   <si>
     <t>MIN</t>
   </si>
@@ -276,13 +276,28 @@
     <t>OK(BS)</t>
   </si>
   <si>
-    <t>NetKu (#tokens)</t>
-  </si>
-  <si>
-    <t>edit_NetKu (#tokens)</t>
-  </si>
-  <si>
-    <t>With [ST] + text + [\ST]</t>
+    <t>non_updated_summary</t>
+  </si>
+  <si>
+    <t>updated_summary</t>
+  </si>
+  <si>
+    <t>Train Set (#paragraphs)</t>
+  </si>
+  <si>
+    <t>(except of trigger)</t>
+  </si>
+  <si>
+    <t># ratios</t>
+  </si>
+  <si>
+    <t>between non_updated, updated</t>
+  </si>
+  <si>
+    <t>485/1602</t>
+  </si>
+  <si>
+    <t>#(&lt;99%)</t>
   </si>
 </sst>
 </file>
@@ -525,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -777,6 +792,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,13 +1114,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="B2:AE202"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="124" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="H173" sqref="H173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.5" customWidth="1"/>
     <col min="10" max="10" width="10.1640625" customWidth="1"/>
@@ -5551,7 +5572,7 @@
     </row>
     <row r="167" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C167" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="D167" s="60"/>
       <c r="E167" s="60"/>
@@ -5559,7 +5580,9 @@
       <c r="G167" s="55"/>
     </row>
     <row r="168" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C168" s="14"/>
+      <c r="C168" s="13" t="s">
+        <v>81</v>
+      </c>
       <c r="D168" s="99" t="s">
         <v>0</v>
       </c>
@@ -5579,16 +5602,19 @@
         <v>79</v>
       </c>
       <c r="D169" s="4">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E169" s="4">
-        <v>30373</v>
+        <v>13</v>
       </c>
       <c r="F169" s="4">
-        <v>4041.9819000000002</v>
+        <v>2.4607000000000001</v>
       </c>
       <c r="G169" s="39">
-        <v>2251</v>
+        <v>2</v>
+      </c>
+      <c r="H169" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="170" spans="3:21" x14ac:dyDescent="0.2">
@@ -5596,16 +5622,16 @@
         <v>80</v>
       </c>
       <c r="D170" s="4">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E170" s="4">
-        <v>35075</v>
+        <v>13</v>
       </c>
       <c r="F170" s="4">
-        <v>4789.3819999999996</v>
+        <v>2.4045000000000001</v>
       </c>
       <c r="G170" s="39">
-        <v>2681</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="3:21" x14ac:dyDescent="0.2">
@@ -5616,28 +5642,53 @@
       <c r="J171" s="55"/>
     </row>
     <row r="172" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="D172" s="16"/>
-      <c r="E172" s="16"/>
-      <c r="F172" s="16"/>
-      <c r="G172" s="16"/>
+      <c r="C172" t="s">
+        <v>83</v>
+      </c>
+      <c r="D172" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="E172" s="99" t="s">
+        <v>1</v>
+      </c>
+      <c r="F172" s="99" t="s">
+        <v>2</v>
+      </c>
+      <c r="G172" s="99" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="173" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C173" s="72"/>
-      <c r="D173" s="66"/>
-      <c r="E173" s="66"/>
-      <c r="F173" s="66"/>
-      <c r="G173" s="16"/>
+      <c r="D173" s="81">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="E173" s="81">
+        <v>1</v>
+      </c>
+      <c r="F173" s="81">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="G173" s="101">
+        <v>0.99890000000000001</v>
+      </c>
+      <c r="H173" s="102" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="174" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C174" s="50"/>
       <c r="D174" s="52"/>
       <c r="E174" s="52"/>
       <c r="F174" s="52"/>
       <c r="G174" s="16"/>
     </row>
     <row r="175" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C175" s="71"/>
-      <c r="D175" s="51"/>
+      <c r="C175" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="D175" s="51" t="s">
+        <v>85</v>
+      </c>
       <c r="E175" s="51"/>
       <c r="F175" s="51"/>
       <c r="G175" s="16"/>

</xml_diff>

<commit_message>
Update progress before meeting
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BADCBA-D735-5245-9012-4478AA5AF37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07624EC9-ED09-C644-AADE-5058D5DD25FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="88">
   <si>
     <t>MIN</t>
   </si>
@@ -285,9 +285,6 @@
     <t>Train Set (#paragraphs)</t>
   </si>
   <si>
-    <t>(except of trigger)</t>
-  </si>
-  <si>
     <t># ratios</t>
   </si>
   <si>
@@ -298,6 +295,12 @@
   </si>
   <si>
     <t>#(&lt;99%)</t>
+  </si>
+  <si>
+    <t>remove trigger</t>
+  </si>
+  <si>
+    <t>trigger removed</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="B2:AE202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="124" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="H173" sqref="H173"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D175" sqref="D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5614,7 +5617,7 @@
         <v>2</v>
       </c>
       <c r="H169" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
     </row>
     <row r="170" spans="3:21" x14ac:dyDescent="0.2">
@@ -5632,6 +5635,9 @@
       </c>
       <c r="G170" s="39">
         <v>2</v>
+      </c>
+      <c r="H170" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="171" spans="3:21" x14ac:dyDescent="0.2">
@@ -5643,7 +5649,7 @@
     </row>
     <row r="172" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C172" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D172" s="99" t="s">
         <v>0</v>
@@ -5659,7 +5665,9 @@
       </c>
     </row>
     <row r="173" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C173" s="72"/>
+      <c r="C173" t="s">
+        <v>87</v>
+      </c>
       <c r="D173" s="81">
         <v>4.9000000000000002E-2</v>
       </c>
@@ -5673,7 +5681,7 @@
         <v>0.99890000000000001</v>
       </c>
       <c r="H173" s="102" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="174" spans="3:21" x14ac:dyDescent="0.2">
@@ -5684,10 +5692,10 @@
     </row>
     <row r="175" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C175" s="50" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D175" s="51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E175" s="51"/>
       <c r="F175" s="51"/>

</xml_diff>

<commit_message>
Update progress and todo after discussion with Prof. Huang
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07624EC9-ED09-C644-AADE-5058D5DD25FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1AD2BC-B240-6146-86B3-6C44997A7C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="90">
   <si>
     <t>MIN</t>
   </si>
@@ -297,10 +297,16 @@
     <t>#(&lt;99%)</t>
   </si>
   <si>
-    <t>remove trigger</t>
-  </si>
-  <si>
     <t>trigger removed</t>
+  </si>
+  <si>
+    <t>calculate</t>
+  </si>
+  <si>
+    <t>diff on train set [RM], [ADD], [SUB]</t>
+  </si>
+  <si>
+    <t>From Our Paper</t>
   </si>
 </sst>
 </file>
@@ -1117,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="B2:AE202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D175" sqref="D175"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="200" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5616,7 +5622,7 @@
       <c r="G169" s="39">
         <v>2</v>
       </c>
-      <c r="H169" t="s">
+      <c r="H169" s="44" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5636,7 +5642,7 @@
       <c r="G170" s="39">
         <v>2</v>
       </c>
-      <c r="H170" t="s">
+      <c r="H170" s="44" t="s">
         <v>86</v>
       </c>
     </row>
@@ -5666,7 +5672,7 @@
     </row>
     <row r="173" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D173" s="81">
         <v>4.9000000000000002E-2</v>
@@ -5704,15 +5710,23 @@
     <row r="176" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C176" s="72"/>
       <c r="D176" s="16"/>
-      <c r="E176" s="16"/>
-      <c r="F176" s="16"/>
+      <c r="E176" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F176" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="G176" s="16"/>
     </row>
     <row r="177" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C177" s="16"/>
       <c r="D177" s="16"/>
-      <c r="E177" s="16"/>
-      <c r="F177" s="16"/>
+      <c r="E177" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F177" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="G177" s="16"/>
     </row>
     <row r="178" spans="3:18" x14ac:dyDescent="0.2">
@@ -5730,18 +5744,38 @@
       <c r="G179" s="16"/>
     </row>
     <row r="180" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C180" s="50"/>
-      <c r="D180" s="60"/>
-      <c r="E180" s="60"/>
-      <c r="F180" s="60"/>
-      <c r="G180" s="16"/>
+      <c r="C180" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="D180" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="E180" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G180" s="54" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="181" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C181" s="71"/>
-      <c r="D181" s="60"/>
-      <c r="E181" s="60"/>
-      <c r="F181" s="60"/>
-      <c r="G181" s="16"/>
+      <c r="C181" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D181" s="49">
+        <v>0.93359999999999999</v>
+      </c>
+      <c r="E181" s="49">
+        <v>0.91759999999999997</v>
+      </c>
+      <c r="F181" s="49">
+        <v>0.93320000000000003</v>
+      </c>
+      <c r="G181" s="58">
+        <v>0.98399999999999999</v>
+      </c>
     </row>
     <row r="182" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C182" s="65"/>

</xml_diff>

<commit_message>
Update README for train_examine
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E1E1E4-71BF-9F45-AC6E-9F46F9920EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A514C5-800D-7B41-A93A-CB18A7874B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Done with calculate the edits actions from train set in summary-level without trigger existed
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A514C5-800D-7B41-A93A-CB18A7874B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F96CDDF-2E79-F24E-8CFA-2C91F4EE7B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="92">
   <si>
     <t>MIN</t>
   </si>
@@ -300,22 +300,19 @@
     <t>trigger removed</t>
   </si>
   <si>
-    <t>calculate</t>
-  </si>
-  <si>
-    <t>diff on train set [RM], [ADD], [SUB]</t>
-  </si>
-  <si>
     <t>From Our Paper</t>
   </si>
   <si>
-    <t>create new version of train set without trigger for computing</t>
-  </si>
-  <si>
     <t>Re-calculate</t>
   </si>
   <si>
     <t>Ground Truth without trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Actions </t>
+  </si>
+  <si>
+    <t>(#ADD+#SUB+#RM)</t>
   </si>
 </sst>
 </file>
@@ -558,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -822,6 +819,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1139,14 +1146,14 @@
   <dimension ref="B2:AE202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A161" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F179" sqref="F179"/>
+      <selection activeCell="D187" sqref="D187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="0.1640625" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.5" customWidth="1"/>
     <col min="10" max="10" width="10.1640625" customWidth="1"/>
@@ -5727,27 +5734,16 @@
     <row r="176" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C176" s="71"/>
       <c r="D176" s="16"/>
-      <c r="E176" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F176" s="16" t="s">
-        <v>16</v>
-      </c>
+      <c r="E176" s="16"/>
+      <c r="F176" s="16"/>
       <c r="G176" s="16"/>
     </row>
     <row r="177" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C177" s="16"/>
       <c r="D177" s="16"/>
-      <c r="E177" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="F177" s="16" t="s">
-        <v>88</v>
-      </c>
+      <c r="E177" s="16"/>
+      <c r="F177" s="16"/>
       <c r="G177" s="16"/>
-      <c r="J177" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="178" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C178" s="16"/>
@@ -5765,7 +5761,7 @@
     </row>
     <row r="180" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C180" s="87" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D180" s="46" t="s">
         <v>14</v>
@@ -5782,7 +5778,7 @@
     </row>
     <row r="181" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C181" s="45" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D181" s="49">
         <v>0.93359999999999999</v>
@@ -5799,7 +5795,7 @@
     </row>
     <row r="182" spans="3:18" x14ac:dyDescent="0.2">
       <c r="C182" s="102" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D182" s="103">
         <v>0.96809999999999996</v>
@@ -5830,16 +5826,38 @@
       <c r="R183" s="16"/>
     </row>
     <row r="184" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C184" s="71"/>
-      <c r="D184" s="16"/>
-      <c r="E184" s="16"/>
-      <c r="F184" s="16"/>
+      <c r="C184" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="D184" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="E184" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="F184" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="G184" s="98" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="185" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C185" s="16"/>
-      <c r="D185" s="16"/>
-      <c r="E185" s="16"/>
-      <c r="F185" s="16"/>
+      <c r="C185" s="108" t="s">
+        <v>91</v>
+      </c>
+      <c r="D185" s="105">
+        <v>0</v>
+      </c>
+      <c r="E185" s="105">
+        <v>14</v>
+      </c>
+      <c r="F185" s="105">
+        <v>1.3021</v>
+      </c>
+      <c r="G185" s="106">
+        <v>0</v>
+      </c>
       <c r="N185" s="70"/>
       <c r="O185" s="65"/>
       <c r="P185" s="65"/>

</xml_diff>

<commit_message>
Update baseline and todo
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F96CDDF-2E79-F24E-8CFA-2C91F4EE7B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAC5AF9-4A15-CA4B-BFAA-BCB1A6B21DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="96">
   <si>
     <t>MIN</t>
   </si>
@@ -313,6 +313,18 @@
   </si>
   <si>
     <t>(#ADD+#SUB+#RM)</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Full Content</t>
+  </si>
+  <si>
+    <t>#paragraph</t>
+  </si>
+  <si>
+    <t>Train Set (#paragraphs) diff</t>
   </si>
 </sst>
 </file>
@@ -326,7 +338,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,6 +382,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -555,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -829,6 +855,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="B2:AE202"/>
+  <dimension ref="A2:AE202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D187" sqref="D187"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5473,7 +5506,7 @@
       <c r="Q160" s="41"/>
       <c r="R160" s="41"/>
     </row>
-    <row r="161" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C161" s="87" t="s">
         <v>58</v>
       </c>
@@ -5505,7 +5538,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C162" s="45" t="s">
         <v>65</v>
       </c>
@@ -5540,7 +5573,7 @@
         <v>0.97899999999999998</v>
       </c>
     </row>
-    <row r="163" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C163" s="45" t="s">
         <v>72</v>
       </c>
@@ -5575,7 +5608,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="165" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C165" s="64"/>
       <c r="D165" s="64"/>
       <c r="E165" s="64"/>
@@ -5596,14 +5629,18 @@
       <c r="T165" s="64"/>
       <c r="U165" s="64"/>
     </row>
-    <row r="166" spans="3:21" x14ac:dyDescent="0.2">
-      <c r="C166" s="71"/>
+    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A166" s="109"/>
+      <c r="B166" s="109"/>
+      <c r="C166" s="110" t="s">
+        <v>92</v>
+      </c>
       <c r="D166" s="65"/>
       <c r="E166" s="65"/>
       <c r="F166" s="65"/>
       <c r="G166" s="16"/>
     </row>
-    <row r="167" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C167" t="s">
         <v>4</v>
       </c>
@@ -5612,7 +5649,7 @@
       <c r="F167" s="60"/>
       <c r="G167" s="55"/>
     </row>
-    <row r="168" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C168" s="13" t="s">
         <v>81</v>
       </c>
@@ -5630,7 +5667,7 @@
       </c>
       <c r="J168" s="55"/>
     </row>
-    <row r="169" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C169" s="99" t="s">
         <v>79</v>
       </c>
@@ -5650,7 +5687,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C170" s="13" t="s">
         <v>80</v>
       </c>
@@ -5670,14 +5707,14 @@
         <v>86</v>
       </c>
     </row>
-    <row r="171" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D171" s="16"/>
       <c r="E171" s="16"/>
       <c r="F171" s="16"/>
       <c r="G171" s="16"/>
       <c r="J171" s="55"/>
     </row>
-    <row r="172" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C172" t="s">
         <v>82</v>
       </c>
@@ -5694,7 +5731,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
         <v>86</v>
       </c>
@@ -5714,13 +5751,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="174" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D174" s="52"/>
       <c r="E174" s="52"/>
       <c r="F174" s="52"/>
       <c r="G174" s="16"/>
     </row>
-    <row r="175" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C175" s="50" t="s">
         <v>85</v>
       </c>
@@ -5731,7 +5768,7 @@
       <c r="F175" s="51"/>
       <c r="G175" s="16"/>
     </row>
-    <row r="176" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
       <c r="C176" s="71"/>
       <c r="D176" s="16"/>
       <c r="E176" s="16"/>
@@ -5871,8 +5908,55 @@
       <c r="Q186" s="60"/>
       <c r="R186" s="62"/>
     </row>
+    <row r="187" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C187" s="110" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="188" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C188" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="189" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C189" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D189" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="E189" s="98" t="s">
+        <v>1</v>
+      </c>
+      <c r="F189" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="G189" s="98" t="s">
+        <v>3</v>
+      </c>
       <c r="J189" s="55"/>
+    </row>
+    <row r="190" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C190" s="99"/>
+      <c r="D190" s="4">
+        <v>0</v>
+      </c>
+      <c r="E190" s="4">
+        <v>20</v>
+      </c>
+      <c r="F190" s="4">
+        <v>0.78959999999999997</v>
+      </c>
+      <c r="G190" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="3:18" x14ac:dyDescent="0.2">
+      <c r="C191" s="50"/>
+      <c r="D191" s="51"/>
+      <c r="E191" s="51"/>
+      <c r="F191" s="51"/>
+      <c r="G191" s="111"/>
     </row>
     <row r="192" spans="3:18" x14ac:dyDescent="0.2">
       <c r="J192" s="55"/>

</xml_diff>

<commit_message>
Update README and baselines
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAC5AF9-4A15-CA4B-BFAA-BCB1A6B21DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA7259D-70D8-BE40-AA2D-B3A642712BD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="96">
   <si>
     <t>MIN</t>
   </si>
@@ -1178,8 +1178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D191" sqref="D191"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G186" sqref="G186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5790,7 +5790,9 @@
       <c r="G178" s="16"/>
     </row>
     <row r="179" spans="3:18" x14ac:dyDescent="0.2">
-      <c r="C179" s="71"/>
+      <c r="C179" s="110" t="s">
+        <v>93</v>
+      </c>
       <c r="D179" s="65"/>
       <c r="E179" s="65"/>
       <c r="F179" s="65"/>

</xml_diff>

<commit_message>
Update dataset and update the indices for test set
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4C2807-42EB-074D-869D-5A96D5C57621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8916A578-5F60-AB48-8018-EF04A8BD9A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="23500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1174,7 +1174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A179" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H197" sqref="H197"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add labeled #paragraphs for train set
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDE59EB-FC28-0746-B409-D1D2BDB981F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B5CA6E-75FC-BD40-AB4E-CB98EE205794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="8800" yWindow="4400" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$C$4:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="110">
   <si>
     <t>MIN</t>
   </si>
@@ -345,9 +347,6 @@
     <t>Other Sections</t>
   </si>
   <si>
-    <t>True/False</t>
-  </si>
-  <si>
     <t>Paragraph</t>
   </si>
   <si>
@@ -361,6 +360,15 @@
   </si>
   <si>
     <t>Concatenation of x and e</t>
+  </si>
+  <si>
+    <t>0/1</t>
+  </si>
+  <si>
+    <t>#paragraphs:</t>
+  </si>
+  <si>
+    <t>71874/1972</t>
   </si>
 </sst>
 </file>
@@ -1202,7 +1210,7 @@
   <dimension ref="A2:AE202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A177" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H194" sqref="H194"/>
+      <selection activeCell="F195" sqref="F195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5918,10 +5926,10 @@
         <v>96</v>
       </c>
       <c r="D192" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E192" s="94" t="s">
         <v>103</v>
-      </c>
-      <c r="E192" s="94" t="s">
-        <v>104</v>
       </c>
       <c r="F192" s="94" t="s">
         <v>97</v>
@@ -5941,7 +5949,15 @@
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
       <c r="F193" s="98" t="s">
-        <v>102</v>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C194" t="s">
+        <v>108</v>
+      </c>
+      <c r="F194" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.2">
@@ -5954,7 +5970,7 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C198" s="76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D198" s="43" t="s">
         <v>14</v>
@@ -5987,7 +6003,7 @@
     <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B199" s="41"/>
       <c r="C199" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D199" s="46"/>
       <c r="E199" s="46"/>
@@ -6002,7 +6018,7 @@
     <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B200" s="41"/>
       <c r="C200" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>

</xml_diff>

<commit_message>
Update train set and prediction
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B5CA6E-75FC-BD40-AB4E-CB98EE205794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEE2A36-CA1B-4D4E-98C8-48DCB0836D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="4400" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="112">
   <si>
     <t>MIN</t>
   </si>
@@ -347,6 +347,9 @@
     <t>Other Sections</t>
   </si>
   <si>
+    <t>True/False</t>
+  </si>
+  <si>
     <t>Paragraph</t>
   </si>
   <si>
@@ -368,7 +371,10 @@
     <t>#paragraphs:</t>
   </si>
   <si>
-    <t>71874/1972</t>
+    <t>baseline for test set (Ground Truth)</t>
+  </si>
+  <si>
+    <t>1972/71874</t>
   </si>
 </sst>
 </file>
@@ -1207,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="A2:AE202"/>
+  <dimension ref="A2:AE204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F195" sqref="F195"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5926,10 +5932,10 @@
         <v>96</v>
       </c>
       <c r="D192" s="94" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E192" s="94" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F192" s="94" t="s">
         <v>97</v>
@@ -5949,14 +5955,11 @@
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
       <c r="F193" s="98" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C194" t="s">
-        <v>108</v>
-      </c>
-      <c r="F194" t="s">
         <v>109</v>
       </c>
     </row>
@@ -5970,7 +5973,7 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C198" s="76" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D198" s="43" t="s">
         <v>14</v>
@@ -6003,7 +6006,7 @@
     <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B199" s="41"/>
       <c r="C199" s="42" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D199" s="46"/>
       <c r="E199" s="46"/>
@@ -6018,7 +6021,7 @@
     <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B200" s="41"/>
       <c r="C200" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -6037,6 +6040,37 @@
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B202" s="41"/>
+      <c r="C202" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G202" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="E203" s="1">
+        <v>0.98160000000000003</v>
+      </c>
+      <c r="F203" s="1">
+        <v>0.97489999999999999</v>
+      </c>
+      <c r="G203" s="1">
+        <v>0.98140000000000005</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C204" t="s">
+        <v>102</v>
+      </c>
+      <c r="D204" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
Update data: fix the data
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEE2A36-CA1B-4D4E-98C8-48DCB0836D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8981DA63-3F6A-A547-A715-A3EF056AA415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="8800" yWindow="4400" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="115">
   <si>
     <t>MIN</t>
   </si>
@@ -347,9 +347,6 @@
     <t>Other Sections</t>
   </si>
   <si>
-    <t>True/False</t>
-  </si>
-  <si>
     <t>Paragraph</t>
   </si>
   <si>
@@ -375,6 +372,18 @@
   </si>
   <si>
     <t>1972/71874</t>
+  </si>
+  <si>
+    <t>Train set: True/False</t>
+  </si>
+  <si>
+    <t>Test set: True/False</t>
+  </si>
+  <si>
+    <t>Val set: True/False</t>
+  </si>
+  <si>
+    <t>11052/201</t>
   </si>
 </sst>
 </file>
@@ -1213,9 +1222,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="A2:AE204"/>
+  <dimension ref="A2:AE206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="D205" sqref="D205"/>
     </sheetView>
   </sheetViews>
@@ -5932,10 +5941,10 @@
         <v>96</v>
       </c>
       <c r="D192" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E192" s="94" t="s">
         <v>103</v>
-      </c>
-      <c r="E192" s="94" t="s">
-        <v>104</v>
       </c>
       <c r="F192" s="94" t="s">
         <v>97</v>
@@ -5955,12 +5964,12 @@
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
       <c r="F193" s="98" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C194" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.2">
@@ -5973,7 +5982,7 @@
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C198" s="76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D198" s="43" t="s">
         <v>14</v>
@@ -6006,7 +6015,7 @@
     <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B199" s="41"/>
       <c r="C199" s="42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D199" s="46"/>
       <c r="E199" s="46"/>
@@ -6021,7 +6030,7 @@
     <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B200" s="41"/>
       <c r="C200" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D200" s="2"/>
       <c r="E200" s="2"/>
@@ -6041,7 +6050,7 @@
     <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B202" s="41"/>
       <c r="C202" s="41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>14</v>
@@ -6066,10 +6075,23 @@
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="C204" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D204" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C205" t="s">
+        <v>112</v>
+      </c>
+      <c r="D205" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C206" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update classification result at second experitment
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0895CD-C8FB-504C-B5F6-6FAC94861623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7414C7E-BCF4-844D-95EF-5904D114CC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="4400" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1231,7 +1231,7 @@
   <dimension ref="A2:AE207"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A196" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H204" sqref="H204"/>
+      <selection activeCell="D208" sqref="D208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix the alignment betweeen paragraphs and instances
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7414C7E-BCF4-844D-95EF-5904D114CC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F590E-465F-8B4D-80DF-EBB519E91AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="38380" yWindow="5320" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,9 +368,6 @@
     <t>#paragraphs:</t>
   </si>
   <si>
-    <t>baseline for test set (Ground Truth)</t>
-  </si>
-  <si>
     <t>1972/71874</t>
   </si>
   <si>
@@ -380,16 +377,19 @@
     <t>Test set: True/False</t>
   </si>
   <si>
-    <t>Val set: True/False</t>
-  </si>
-  <si>
-    <t>Pred</t>
-  </si>
-  <si>
-    <t>242/10104</t>
-  </si>
-  <si>
     <t>321/10183</t>
+  </si>
+  <si>
+    <t>371/10054</t>
+  </si>
+  <si>
+    <t>Pred: True/False</t>
+  </si>
+  <si>
+    <t>Test Set (Ground Truth)</t>
+  </si>
+  <si>
+    <t>Experiment</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -481,6 +481,11 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times Nw"/>
     </font>
   </fonts>
   <fills count="4">
@@ -666,7 +671,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -914,6 +919,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1228,13 +1234,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="A2:AE207"/>
+  <dimension ref="A2:AE213"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D208" sqref="D208"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C204" sqref="C204"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="0.1640625" customWidth="1"/>
@@ -1261,17 +1267,17 @@
     <col min="27" max="27" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:26">
       <c r="C2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="3:26">
       <c r="C3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:26">
       <c r="C4" s="6"/>
       <c r="D4" s="7" t="s">
         <v>5</v>
@@ -1282,7 +1288,7 @@
       </c>
       <c r="G4" s="9"/>
     </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:26">
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>0</v>
@@ -1297,7 +1303,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:26">
       <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
@@ -1314,7 +1320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:26">
       <c r="C7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1331,13 +1337,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:26">
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:26">
       <c r="C9" s="3"/>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -1348,7 +1354,7 @@
       </c>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:26">
       <c r="C10" s="31"/>
       <c r="D10" s="12" t="s">
         <v>0</v>
@@ -1393,7 +1399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:26">
       <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:26">
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1487,12 +1493,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:26">
       <c r="C13" s="29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:26">
       <c r="C14" s="30"/>
       <c r="O14" s="4" t="s">
         <v>46</v>
@@ -1525,7 +1531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:26">
       <c r="C15" s="17"/>
       <c r="D15" s="2" t="s">
         <v>9</v>
@@ -1566,7 +1572,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:26">
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
         <v>0</v>
@@ -1611,7 +1617,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:31">
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1628,7 +1634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:31">
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:31">
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -1712,7 +1718,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:31">
       <c r="O20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1744,7 +1750,7 @@
         <v>2153</v>
       </c>
     </row>
-    <row r="21" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:31">
       <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
@@ -1761,7 +1767,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:31">
       <c r="C22" s="18" t="s">
         <v>9</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>0.91</v>
       </c>
     </row>
-    <row r="23" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:31">
       <c r="B23" s="60"/>
       <c r="C23" s="60"/>
       <c r="D23" s="60"/>
@@ -1799,7 +1805,7 @@
       <c r="S23" s="60"/>
       <c r="T23" s="60"/>
     </row>
-    <row r="24" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:31">
       <c r="C24" s="38" t="s">
         <v>32</v>
       </c>
@@ -1807,7 +1813,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:31">
       <c r="C25" s="17"/>
       <c r="D25" s="19" t="s">
         <v>26</v>
@@ -1840,7 +1846,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:31">
       <c r="C26" s="23"/>
       <c r="D26" s="23" t="s">
         <v>0</v>
@@ -1883,7 +1889,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="27" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:31">
       <c r="C27" s="25" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="28" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:31">
       <c r="C28" s="27" t="s">
         <v>12</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:31">
       <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:31">
       <c r="C30" s="4" t="s">
         <v>21</v>
       </c>
@@ -2027,7 +2033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:31">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2040,7 +2046,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:31">
       <c r="C32" s="76" t="s">
         <v>26</v>
       </c>
@@ -2073,7 +2079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:25">
       <c r="C33" s="42" t="s">
         <v>65</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="34" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:25">
       <c r="C34" s="42" t="s">
         <v>72</v>
       </c>
@@ -2143,7 +2149,7 @@
         <v>0.96699999999999997</v>
       </c>
     </row>
-    <row r="35" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:25">
       <c r="D35" s="44"/>
       <c r="E35" s="44"/>
       <c r="F35" s="44"/>
@@ -2154,7 +2160,7 @@
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
     </row>
-    <row r="37" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:25">
       <c r="C37" s="38" t="s">
         <v>34</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:25">
       <c r="C38" s="17"/>
       <c r="D38" s="19" t="s">
         <v>26</v>
@@ -2182,7 +2188,7 @@
       </c>
       <c r="R38" s="68"/>
     </row>
-    <row r="39" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:25">
       <c r="C39" s="23"/>
       <c r="D39" s="23" t="s">
         <v>0</v>
@@ -2210,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:25">
       <c r="C40" s="25" t="s">
         <v>11</v>
       </c>
@@ -2242,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:25">
       <c r="C41" s="27" t="s">
         <v>12</v>
       </c>
@@ -2274,7 +2280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:25">
       <c r="C42" s="4" t="s">
         <v>22</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:25">
       <c r="C43" s="4" t="s">
         <v>21</v>
       </c>
@@ -2338,7 +2344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:25">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2350,7 +2356,7 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:25">
       <c r="C45" s="76" t="s">
         <v>26</v>
       </c>
@@ -2403,7 +2409,7 @@
       <c r="X45" s="48"/>
       <c r="Y45" s="48"/>
     </row>
-    <row r="46" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:25">
       <c r="C46" s="42" t="s">
         <v>65</v>
       </c>
@@ -2459,7 +2465,7 @@
       <c r="X46" s="53"/>
       <c r="Y46" s="53"/>
     </row>
-    <row r="47" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:25">
       <c r="C47" s="78" t="s">
         <v>72</v>
       </c>
@@ -2515,7 +2521,7 @@
       <c r="X47" s="53"/>
       <c r="Y47" s="53"/>
     </row>
-    <row r="48" spans="3:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:25">
       <c r="C48" s="81"/>
       <c r="I48" s="48"/>
       <c r="J48" s="48"/>
@@ -2526,7 +2532,7 @@
       <c r="V48" s="48"/>
       <c r="W48" s="48"/>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:23">
       <c r="C49" s="42" t="s">
         <v>64</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:23">
       <c r="C50" s="45" t="s">
         <v>26</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>0.44669999999999999</v>
       </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:23">
       <c r="C51" s="61"/>
       <c r="D51" t="s">
         <v>76</v>
@@ -2681,11 +2687,11 @@
       </c>
       <c r="N51" s="78"/>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:23">
       <c r="C52" s="62"/>
       <c r="N52" s="62"/>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:23">
       <c r="C53" s="76" t="s">
         <v>26</v>
       </c>
@@ -2711,7 +2717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:23">
       <c r="C54" s="62" t="s">
         <v>64</v>
       </c>
@@ -2740,7 +2746,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:23">
       <c r="C55" s="76" t="s">
         <v>75</v>
       </c>
@@ -2769,7 +2775,7 @@
         <v>0.96809999999999996</v>
       </c>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:23">
       <c r="C57" s="38" t="s">
         <v>36</v>
       </c>
@@ -2777,7 +2783,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:23">
       <c r="C58" s="17"/>
       <c r="D58" s="19" t="s">
         <v>26</v>
@@ -2797,7 +2803,7 @@
       </c>
       <c r="R58" s="22"/>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:23">
       <c r="C59" s="23"/>
       <c r="D59" s="23" t="s">
         <v>0</v>
@@ -2825,7 +2831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:23">
       <c r="C60" s="25" t="s">
         <v>11</v>
       </c>
@@ -2857,7 +2863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:23">
       <c r="C61" s="27" t="s">
         <v>12</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:23">
       <c r="B62" s="41"/>
       <c r="C62" s="4" t="s">
         <v>22</v>
@@ -2922,7 +2928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:23">
       <c r="C63" s="4" t="s">
         <v>21</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:23">
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -2966,7 +2972,7 @@
       <c r="Q64" s="1"/>
       <c r="R64" s="1"/>
     </row>
-    <row r="65" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:21">
       <c r="C65" s="76" t="s">
         <v>26</v>
       </c>
@@ -2999,7 +3005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:21">
       <c r="C66" s="42" t="s">
         <v>65</v>
       </c>
@@ -3035,7 +3041,7 @@
         <v>0.98499999999999999</v>
       </c>
     </row>
-    <row r="67" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:21">
       <c r="C67" s="42" t="s">
         <v>72</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>0.96099999999999997</v>
       </c>
     </row>
-    <row r="70" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:21">
       <c r="C70" s="57"/>
       <c r="D70" s="57"/>
       <c r="E70" s="57"/>
@@ -3092,10 +3098,10 @@
       <c r="T70" s="57"/>
       <c r="U70" s="57"/>
     </row>
-    <row r="71" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:21">
       <c r="J71" s="62"/>
     </row>
-    <row r="72" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:21">
       <c r="C72" s="38" t="s">
         <v>44</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:21">
       <c r="C73" s="17"/>
       <c r="D73" s="19" t="s">
         <v>46</v>
@@ -3125,7 +3131,7 @@
       </c>
       <c r="R73" s="22"/>
     </row>
-    <row r="74" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:21">
       <c r="C74" s="23"/>
       <c r="D74" s="23" t="s">
         <v>0</v>
@@ -3153,7 +3159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:21">
       <c r="C75" s="25" t="s">
         <v>11</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:21">
       <c r="C76" s="27" t="s">
         <v>12</v>
       </c>
@@ -3217,7 +3223,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:21">
       <c r="C77" s="4" t="s">
         <v>22</v>
       </c>
@@ -3249,7 +3255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:21">
       <c r="C78" s="4" t="s">
         <v>21</v>
       </c>
@@ -3281,7 +3287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:21">
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -3294,7 +3300,7 @@
       <c r="Q79" s="1"/>
       <c r="R79" s="1"/>
     </row>
-    <row r="80" spans="3:21" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:21">
       <c r="C80" s="76" t="s">
         <v>46</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:23">
       <c r="C81" s="42" t="s">
         <v>65</v>
       </c>
@@ -3362,7 +3368,7 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="82" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:23">
       <c r="C82" s="42" t="s">
         <v>72</v>
       </c>
@@ -3397,13 +3403,13 @@
         <v>0.95499999999999996</v>
       </c>
     </row>
-    <row r="83" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:23">
       <c r="D83" s="44"/>
       <c r="E83" s="44"/>
       <c r="F83" s="44"/>
       <c r="G83" s="44"/>
     </row>
-    <row r="85" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:23">
       <c r="C85" s="38" t="s">
         <v>47</v>
       </c>
@@ -3411,7 +3417,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:23">
       <c r="C86" s="17"/>
       <c r="D86" s="19" t="s">
         <v>46</v>
@@ -3431,7 +3437,7 @@
       </c>
       <c r="R86" s="22"/>
     </row>
-    <row r="87" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:23">
       <c r="C87" s="23"/>
       <c r="D87" s="23" t="s">
         <v>0</v>
@@ -3459,7 +3465,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:23">
       <c r="C88" s="25" t="s">
         <v>11</v>
       </c>
@@ -3491,7 +3497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="3:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:23" ht="17" customHeight="1">
       <c r="C89" s="27" t="s">
         <v>12</v>
       </c>
@@ -3523,7 +3529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:23">
       <c r="C90" s="4" t="s">
         <v>22</v>
       </c>
@@ -3555,7 +3561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:23">
       <c r="C91" s="4" t="s">
         <v>21</v>
       </c>
@@ -3587,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:23">
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -3599,7 +3605,7 @@
       <c r="Q92" s="1"/>
       <c r="R92" s="1"/>
     </row>
-    <row r="93" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:23">
       <c r="C93" s="76" t="s">
         <v>46</v>
       </c>
@@ -3661,7 +3667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:23">
       <c r="C94" s="42" t="s">
         <v>65</v>
       </c>
@@ -3726,7 +3732,7 @@
         <v>0.54779999999999995</v>
       </c>
     </row>
-    <row r="95" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:23">
       <c r="C95" s="42" t="s">
         <v>72</v>
       </c>
@@ -3791,12 +3797,12 @@
         <v>0.54820000000000002</v>
       </c>
     </row>
-    <row r="96" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:23">
       <c r="C96" s="81"/>
       <c r="I96" s="48"/>
       <c r="N96" s="81"/>
     </row>
-    <row r="97" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:24">
       <c r="C97" s="42" t="s">
         <v>64</v>
       </c>
@@ -3859,7 +3865,7 @@
       </c>
       <c r="X97" s="48"/>
     </row>
-    <row r="98" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:24">
       <c r="C98" s="76" t="s">
         <v>46</v>
       </c>
@@ -3921,7 +3927,7 @@
         <v>0.3992</v>
       </c>
     </row>
-    <row r="99" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:24">
       <c r="D99" t="s">
         <v>76</v>
       </c>
@@ -3950,7 +3956,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:24">
       <c r="C100" s="38" t="s">
         <v>73</v>
       </c>
@@ -3958,7 +3964,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="101" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:24">
       <c r="C101" s="42" t="s">
         <v>66</v>
       </c>
@@ -3984,7 +3990,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:24">
       <c r="C102" s="45" t="s">
         <v>46</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>0.98019999999999996</v>
       </c>
     </row>
-    <row r="105" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:24">
       <c r="C105" s="38" t="s">
         <v>48</v>
       </c>
@@ -4024,7 +4030,7 @@
       <c r="V105" s="48"/>
       <c r="W105" s="48"/>
     </row>
-    <row r="106" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:24">
       <c r="C106" s="17"/>
       <c r="D106" s="19" t="s">
         <v>46</v>
@@ -4044,7 +4050,7 @@
       </c>
       <c r="R106" s="22"/>
     </row>
-    <row r="107" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:24">
       <c r="C107" s="23"/>
       <c r="D107" s="23" t="s">
         <v>0</v>
@@ -4072,7 +4078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:24">
       <c r="C108" s="25" t="s">
         <v>11</v>
       </c>
@@ -4104,7 +4110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:24">
       <c r="C109" s="27" t="s">
         <v>12</v>
       </c>
@@ -4136,7 +4142,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:24">
       <c r="C110" s="4" t="s">
         <v>22</v>
       </c>
@@ -4169,7 +4175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:24">
       <c r="C111" s="4" t="s">
         <v>21</v>
       </c>
@@ -4201,14 +4207,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:24">
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:22">
       <c r="C113" s="76" t="s">
         <v>46</v>
       </c>
@@ -4240,7 +4246,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="114" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:22">
       <c r="C114" s="42" t="s">
         <v>65</v>
       </c>
@@ -4276,7 +4282,7 @@
       </c>
       <c r="U114" s="53"/>
     </row>
-    <row r="115" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:22">
       <c r="C115" s="42" t="s">
         <v>72</v>
       </c>
@@ -4312,7 +4318,7 @@
       </c>
       <c r="T115" s="53"/>
     </row>
-    <row r="118" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:22">
       <c r="C118" s="57"/>
       <c r="D118" s="57"/>
       <c r="E118" s="57"/>
@@ -4333,7 +4339,7 @@
       <c r="T118" s="57"/>
       <c r="U118" s="57"/>
     </row>
-    <row r="120" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:22">
       <c r="C120" s="38" t="s">
         <v>52</v>
       </c>
@@ -4341,7 +4347,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="121" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:22">
       <c r="C121" s="17"/>
       <c r="D121" s="19" t="s">
         <v>58</v>
@@ -4361,7 +4367,7 @@
       </c>
       <c r="R121" s="22"/>
     </row>
-    <row r="122" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:22">
       <c r="C122" s="23"/>
       <c r="D122" s="23" t="s">
         <v>0</v>
@@ -4389,7 +4395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="123" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:22">
       <c r="C123" s="25" t="s">
         <v>11</v>
       </c>
@@ -4421,7 +4427,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="124" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:22">
       <c r="C124" s="27" t="s">
         <v>12</v>
       </c>
@@ -4453,7 +4459,7 @@
         <v>92.5</v>
       </c>
     </row>
-    <row r="125" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:22">
       <c r="C125" s="4" t="s">
         <v>22</v>
       </c>
@@ -4485,7 +4491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:22">
       <c r="C126" s="4" t="s">
         <v>21</v>
       </c>
@@ -4519,7 +4525,7 @@
       <c r="U126" s="53"/>
       <c r="V126" s="55"/>
     </row>
-    <row r="127" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:22">
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
@@ -4532,7 +4538,7 @@
       <c r="Q127" s="1"/>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="2:22" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:22">
       <c r="B128" s="41"/>
       <c r="C128" s="2" t="s">
         <v>58</v>
@@ -4565,7 +4571,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="129" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:23">
       <c r="B129" s="41"/>
       <c r="C129" s="42" t="s">
         <v>65</v>
@@ -4604,7 +4610,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="130" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:23">
       <c r="B130" s="41"/>
       <c r="C130" s="42" t="s">
         <v>72</v>
@@ -4644,13 +4650,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:23">
       <c r="B131" s="41"/>
     </row>
-    <row r="132" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:23">
       <c r="P132" s="53"/>
     </row>
-    <row r="133" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:23">
       <c r="C133" s="38" t="s">
         <v>53</v>
       </c>
@@ -4658,7 +4664,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="134" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:23">
       <c r="C134" s="17"/>
       <c r="D134" s="19" t="s">
         <v>58</v>
@@ -4679,7 +4685,7 @@
       </c>
       <c r="R134" s="22"/>
     </row>
-    <row r="135" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:23">
       <c r="C135" s="23"/>
       <c r="D135" s="23" t="s">
         <v>0</v>
@@ -4707,7 +4713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:23">
       <c r="C136" s="25" t="s">
         <v>11</v>
       </c>
@@ -4739,7 +4745,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="137" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:23">
       <c r="C137" s="27" t="s">
         <v>12</v>
       </c>
@@ -4771,7 +4777,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="138" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:23">
       <c r="C138" s="4" t="s">
         <v>22</v>
       </c>
@@ -4803,7 +4809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:23">
       <c r="C139" s="12" t="s">
         <v>21</v>
       </c>
@@ -4835,7 +4841,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:23">
       <c r="C140" s="34"/>
       <c r="D140" s="34" t="s">
         <v>76</v>
@@ -4867,7 +4873,7 @@
       <c r="Q140" s="34"/>
       <c r="R140" s="34"/>
     </row>
-    <row r="141" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:23">
       <c r="C141" s="76" t="s">
         <v>58</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="142" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:23">
       <c r="C142" s="42" t="s">
         <v>65</v>
       </c>
@@ -4991,7 +4997,7 @@
         <v>0.73509999999999998</v>
       </c>
     </row>
-    <row r="143" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:23">
       <c r="C143" s="42" t="s">
         <v>72</v>
       </c>
@@ -5053,7 +5059,7 @@
         <v>0.6996</v>
       </c>
     </row>
-    <row r="144" spans="2:23" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:23">
       <c r="C144" s="81"/>
       <c r="D144" t="s">
         <v>76</v>
@@ -5084,11 +5090,11 @@
       </c>
       <c r="N144" s="81"/>
     </row>
-    <row r="145" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:23">
       <c r="C145" s="61"/>
       <c r="N145" s="61"/>
     </row>
-    <row r="146" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:23">
       <c r="C146" s="42" t="s">
         <v>64</v>
       </c>
@@ -5150,7 +5156,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="147" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:23">
       <c r="C147" s="45" t="s">
         <v>58</v>
       </c>
@@ -5212,7 +5218,7 @@
         <v>0.54110000000000003</v>
       </c>
     </row>
-    <row r="148" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:23">
       <c r="D148" t="s">
         <v>76</v>
       </c>
@@ -5256,7 +5262,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="149" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:23">
       <c r="C149" s="38" t="s">
         <v>62</v>
       </c>
@@ -5264,7 +5270,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="150" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:23">
       <c r="C150" s="42" t="s">
         <v>66</v>
       </c>
@@ -5290,7 +5296,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:23">
       <c r="C151" s="45" t="s">
         <v>58</v>
       </c>
@@ -5319,7 +5325,7 @@
         <v>0.47910000000000003</v>
       </c>
     </row>
-    <row r="153" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:23">
       <c r="C153" s="38" t="s">
         <v>54</v>
       </c>
@@ -5327,7 +5333,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="154" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:23">
       <c r="C154" s="17"/>
       <c r="D154" s="19" t="s">
         <v>58</v>
@@ -5347,7 +5353,7 @@
       </c>
       <c r="R154" s="22"/>
     </row>
-    <row r="155" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:23">
       <c r="C155" s="23"/>
       <c r="D155" s="23" t="s">
         <v>0</v>
@@ -5375,7 +5381,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:23">
       <c r="C156" s="25" t="s">
         <v>11</v>
       </c>
@@ -5407,7 +5413,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="157" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:23">
       <c r="C157" s="27" t="s">
         <v>12</v>
       </c>
@@ -5439,7 +5445,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="158" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:23">
       <c r="C158" s="4" t="s">
         <v>22</v>
       </c>
@@ -5471,7 +5477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:23">
       <c r="C159" s="12" t="s">
         <v>21</v>
       </c>
@@ -5503,7 +5509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:23">
       <c r="C160" s="34"/>
       <c r="D160" s="34"/>
       <c r="E160" s="34"/>
@@ -5515,7 +5521,7 @@
       <c r="Q160" s="34"/>
       <c r="R160" s="34"/>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:21">
       <c r="C161" s="76" t="s">
         <v>58</v>
       </c>
@@ -5547,7 +5553,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:21">
       <c r="C162" s="42" t="s">
         <v>65</v>
       </c>
@@ -5582,7 +5588,7 @@
         <v>0.97899999999999998</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:21">
       <c r="C163" s="42" t="s">
         <v>72</v>
       </c>
@@ -5617,7 +5623,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:21">
       <c r="C165" s="57"/>
       <c r="D165" s="57"/>
       <c r="E165" s="57"/>
@@ -5638,7 +5644,7 @@
       <c r="T165" s="57"/>
       <c r="U165" s="57"/>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:21">
       <c r="A166" s="92"/>
       <c r="B166" s="92"/>
       <c r="C166" s="93" t="s">
@@ -5648,7 +5654,7 @@
       <c r="E166" s="48"/>
       <c r="F166" s="48"/>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:21">
       <c r="C167" t="s">
         <v>4</v>
       </c>
@@ -5657,7 +5663,7 @@
       <c r="F167" s="53"/>
       <c r="G167" s="48"/>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:21">
       <c r="C168" s="13" t="s">
         <v>81</v>
       </c>
@@ -5675,7 +5681,7 @@
       </c>
       <c r="J168" s="48"/>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:21">
       <c r="C169" s="86" t="s">
         <v>79</v>
       </c>
@@ -5695,7 +5701,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:21">
       <c r="C170" s="13" t="s">
         <v>80</v>
       </c>
@@ -5715,10 +5721,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:21">
       <c r="J171" s="48"/>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:21">
       <c r="C172" t="s">
         <v>82</v>
       </c>
@@ -5735,7 +5741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:21">
       <c r="C173" t="s">
         <v>86</v>
       </c>
@@ -5755,12 +5761,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:21">
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
       <c r="F174" s="1"/>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:21">
       <c r="C175" s="41" t="s">
         <v>85</v>
       </c>
@@ -5770,16 +5776,16 @@
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:21">
       <c r="C176" s="62"/>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:18">
       <c r="C179" s="93"/>
       <c r="D179" s="48"/>
       <c r="E179" s="48"/>
       <c r="F179" s="48"/>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:18">
       <c r="C180" s="76" t="s">
         <v>87</v>
       </c>
@@ -5796,7 +5802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:18">
       <c r="C181" s="42" t="s">
         <v>89</v>
       </c>
@@ -5813,7 +5819,7 @@
         <v>0.98399999999999999</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:18">
       <c r="C182" s="87" t="s">
         <v>88</v>
       </c>
@@ -5834,13 +5840,13 @@
       <c r="Q182" s="48"/>
       <c r="R182" s="48"/>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:18">
       <c r="D183" s="48"/>
       <c r="E183" s="48"/>
       <c r="F183" s="48"/>
       <c r="I183" s="53"/>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:18">
       <c r="C184" s="90" t="s">
         <v>90</v>
       </c>
@@ -5857,7 +5863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:18">
       <c r="C185" s="91" t="s">
         <v>91</v>
       </c>
@@ -5879,24 +5885,24 @@
       <c r="Q185" s="48"/>
       <c r="R185" s="48"/>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:18">
       <c r="N186" s="62"/>
       <c r="O186" s="53"/>
       <c r="P186" s="53"/>
       <c r="Q186" s="53"/>
       <c r="R186" s="55"/>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:18">
       <c r="C187" s="93" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:18">
       <c r="C188" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:18">
       <c r="C189" s="13" t="s">
         <v>95</v>
       </c>
@@ -5914,7 +5920,7 @@
       </c>
       <c r="J189" s="48"/>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:18">
       <c r="C190" s="86"/>
       <c r="D190" s="4">
         <v>0</v>
@@ -5929,7 +5935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:18">
       <c r="C191" s="99"/>
       <c r="D191" s="100"/>
       <c r="E191" s="100"/>
@@ -5939,7 +5945,7 @@
       <c r="I191" s="57"/>
       <c r="J191" s="57"/>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:18">
       <c r="A192" s="92" t="s">
         <v>98</v>
       </c>
@@ -5965,7 +5971,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18">
       <c r="C193" s="14"/>
       <c r="D193" s="14"/>
       <c r="E193" s="14"/>
@@ -5973,12 +5979,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:18">
       <c r="C194" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:18">
       <c r="A195" s="92" t="s">
         <v>99</v>
       </c>
@@ -5986,7 +5992,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:18">
       <c r="C198" s="76" t="s">
         <v>105</v>
       </c>
@@ -6018,7 +6024,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18">
       <c r="B199" s="41"/>
       <c r="C199" s="42" t="s">
         <v>104</v>
@@ -6033,7 +6039,7 @@
       <c r="K199" s="8"/>
       <c r="L199" s="8"/>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:18">
       <c r="B200" s="41"/>
       <c r="C200" s="7" t="s">
         <v>106</v>
@@ -6049,63 +6055,67 @@
       <c r="L200" s="8"/>
       <c r="R200" s="48"/>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18">
       <c r="B201" s="41"/>
       <c r="R201" s="55"/>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18">
       <c r="B202" s="41"/>
-      <c r="C202" s="41" t="s">
+      <c r="D202" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E202" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:18">
+      <c r="C203" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D203" s="1">
+        <v>0.98160000000000003</v>
+      </c>
+      <c r="E203" s="1">
+        <v>0.97489999999999999</v>
+      </c>
+      <c r="F203" s="1">
+        <v>0.98140000000000005</v>
+      </c>
+    </row>
+    <row r="204" spans="1:18">
+      <c r="C204" s="41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="210" spans="3:4">
+      <c r="C210" s="103"/>
+      <c r="D210" s="103"/>
+    </row>
+    <row r="211" spans="3:4">
+      <c r="C211" s="103" t="s">
+        <v>110</v>
+      </c>
+      <c r="D211" s="103" t="s">
         <v>109</v>
       </c>
-      <c r="E202" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F202" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G202" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="E203" s="1">
-        <v>0.98160000000000003</v>
-      </c>
-      <c r="F203" s="1">
-        <v>0.97489999999999999</v>
-      </c>
-      <c r="G203" s="1">
-        <v>0.98140000000000005</v>
-      </c>
-    </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C204" t="s">
+    </row>
+    <row r="212" spans="3:4">
+      <c r="C212" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="D204" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C205" t="s">
+      <c r="D212" s="103" t="s">
         <v>112</v>
       </c>
-      <c r="D205" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C206" t="s">
+    </row>
+    <row r="213" spans="3:4">
+      <c r="C213" s="103" t="s">
+        <v>114</v>
+      </c>
+      <c r="D213" s="103" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C207" t="s">
-        <v>114</v>
-      </c>
-      <c r="D207" t="s">
-        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update baselines and experiment results
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034F590E-465F-8B4D-80DF-EBB519E91AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10197C7-7840-0E4C-996F-3B0E5E9936CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38380" yWindow="5320" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="121">
   <si>
     <t>MIN</t>
   </si>
@@ -389,7 +389,19 @@
     <t>Test Set (Ground Truth)</t>
   </si>
   <si>
-    <t>Experiment</t>
+    <t>PRIMERA (fine-tuned)</t>
+  </si>
+  <si>
+    <t>PRIMERA (zero-shot)</t>
+  </si>
+  <si>
+    <t>BART (two-staged)</t>
+  </si>
+  <si>
+    <t>PRIMERA (decoder)</t>
+  </si>
+  <si>
+    <t>ChatGPT (decoder)</t>
   </si>
 </sst>
 </file>
@@ -671,7 +683,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -916,10 +928,12 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1234,10 +1248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="A2:AE213"/>
+  <dimension ref="A2:AE219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C204" sqref="C204"/>
+    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G215" sqref="G215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6005,22 +6019,22 @@
       <c r="F198" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G198" s="102" t="s">
+      <c r="G198" s="103" t="s">
         <v>27</v>
       </c>
-      <c r="H198" s="102" t="s">
+      <c r="H198" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="I198" s="102" t="s">
+      <c r="I198" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="J198" s="102" t="s">
+      <c r="J198" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="K198" s="102" t="s">
+      <c r="K198" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="L198" s="102" t="s">
+      <c r="L198" s="103" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6061,60 +6075,100 @@
     </row>
     <row r="202" spans="1:18">
       <c r="B202" s="41"/>
-      <c r="D202" s="1" t="s">
+    </row>
+    <row r="204" spans="1:18">
+      <c r="C204" s="102"/>
+      <c r="D204" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E202" s="1" t="s">
+      <c r="E204" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="F202" s="1" t="s">
+      <c r="F204" s="34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="203" spans="1:18">
-      <c r="C203" s="41" t="s">
+    <row r="205" spans="1:18">
+      <c r="C205" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D203" s="1">
+      <c r="D205" s="2">
         <v>0.98160000000000003</v>
       </c>
-      <c r="E203" s="1">
+      <c r="E205" s="2">
         <v>0.97489999999999999</v>
       </c>
-      <c r="F203" s="1">
+      <c r="F205" s="2">
         <v>0.98140000000000005</v>
       </c>
     </row>
-    <row r="204" spans="1:18">
-      <c r="C204" s="41" t="s">
+    <row r="206" spans="1:18">
+      <c r="C206" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D206" s="7"/>
+      <c r="E206" s="7"/>
+      <c r="F206" s="7"/>
+    </row>
+    <row r="207" spans="1:18">
+      <c r="C207" s="7" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="210" spans="3:4">
-      <c r="C210" s="103"/>
-      <c r="D210" s="103"/>
-    </row>
-    <row r="211" spans="3:4">
-      <c r="C211" s="103" t="s">
+      <c r="D207" s="7"/>
+      <c r="E207" s="7"/>
+      <c r="F207" s="7"/>
+    </row>
+    <row r="208" spans="1:18">
+      <c r="C208" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="D208" s="89">
+        <v>0.95309999999999995</v>
+      </c>
+      <c r="E208" s="89">
+        <v>0.88529999999999998</v>
+      </c>
+      <c r="F208" s="89">
+        <v>0.95309999999999995</v>
+      </c>
+    </row>
+    <row r="209" spans="3:6">
+      <c r="C209" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D209" s="8"/>
+      <c r="E209" s="8"/>
+      <c r="F209" s="8"/>
+    </row>
+    <row r="210" spans="3:6">
+      <c r="C210" s="105" t="s">
+        <v>120</v>
+      </c>
+      <c r="D210" s="8"/>
+      <c r="E210" s="8"/>
+      <c r="F210" s="8"/>
+    </row>
+    <row r="217" spans="3:6">
+      <c r="C217" s="104" t="s">
         <v>110</v>
       </c>
-      <c r="D211" s="103" t="s">
+      <c r="D217" s="104" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="212" spans="3:4">
-      <c r="C212" s="103" t="s">
+    <row r="218" spans="3:6">
+      <c r="C218" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="D212" s="103" t="s">
+      <c r="D218" s="104" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="213" spans="3:4">
-      <c r="C213" s="103" t="s">
+    <row r="219" spans="3:6">
+      <c r="C219" s="104" t="s">
         <v>114</v>
       </c>
-      <c r="D213" s="103" t="s">
+      <c r="D219" s="104" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ChatGPT results and data
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A277CF-EDDD-8341-B483-1EFB61178672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BECBE09-814B-3442-B750-ECFF73D9FB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1250,8 +1250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G215" sqref="G215"/>
+    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="G210" sqref="G210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6123,13 +6123,13 @@
         <v>118</v>
       </c>
       <c r="D208" s="89">
-        <v>0.95309999999999995</v>
+        <v>0.93059999999999998</v>
       </c>
       <c r="E208" s="89">
-        <v>0.88529999999999998</v>
+        <v>0.86650000000000005</v>
       </c>
       <c r="F208" s="89">
-        <v>0.95309999999999995</v>
+        <v>0.93059999999999998</v>
       </c>
     </row>
     <row r="209" spans="3:6">
@@ -6144,9 +6144,15 @@
       <c r="C210" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="D210" s="8"/>
-      <c r="E210" s="8"/>
-      <c r="F210" s="8"/>
+      <c r="D210" s="2">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="E210" s="2">
+        <v>0.8367</v>
+      </c>
+      <c r="F210" s="2">
+        <v>0.88229999999999997</v>
+      </c>
     </row>
     <row r="217" spans="3:6">
       <c r="C217" s="104" t="s">

</xml_diff>

<commit_message>
Update progress and baselines
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CAA998-511B-B240-B784-82F6B09BF001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B1184-7830-DE49-A0E6-37743D5861EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="124">
   <si>
     <t>MIN</t>
   </si>
@@ -410,13 +410,7 @@
     <t>Edit</t>
   </si>
   <si>
-    <t>feed the all paragraphs to chatgpt api</t>
-  </si>
-  <si>
-    <t>let the chatgpt to edit</t>
-  </si>
-  <si>
-    <t>remove the instance which cannot feed into chatgpt. When calculate with our experiments, remove those instances which cannot feed into chatgpt</t>
+    <t>ChatGPT (two-staged)</t>
   </si>
 </sst>
 </file>
@@ -698,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -930,8 +924,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,11 +938,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1266,15 +1256,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C215" sqref="C215"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D211" sqref="D211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="0.1640625" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
@@ -6041,22 +6031,22 @@
       <c r="F198" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G198" s="103" t="s">
+      <c r="G198" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="H198" s="103" t="s">
+      <c r="H198" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="I198" s="103" t="s">
+      <c r="I198" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="J198" s="103" t="s">
+      <c r="J198" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="K198" s="103" t="s">
+      <c r="K198" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="L198" s="103" t="s">
+      <c r="L198" s="43" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6098,120 +6088,128 @@
     <row r="202" spans="1:18">
       <c r="B202" s="41"/>
     </row>
+    <row r="203" spans="1:18">
+      <c r="C203" s="102"/>
+      <c r="D203" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E203" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="F203" s="34" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="204" spans="1:18">
-      <c r="C204" s="102"/>
-      <c r="D204" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="E204" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="F204" s="34" t="s">
-        <v>16</v>
+      <c r="C204" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D204" s="2">
+        <v>0.98160000000000003</v>
+      </c>
+      <c r="E204" s="2">
+        <v>0.97489999999999999</v>
+      </c>
+      <c r="F204" s="2">
+        <v>0.98140000000000005</v>
       </c>
     </row>
     <row r="205" spans="1:18">
       <c r="C205" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D205" s="2">
-        <v>0.98160000000000003</v>
-      </c>
-      <c r="E205" s="2">
-        <v>0.97489999999999999</v>
-      </c>
-      <c r="F205" s="2">
-        <v>0.98140000000000005</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
     </row>
     <row r="206" spans="1:18">
       <c r="C206" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D206" s="7"/>
       <c r="E206" s="7"/>
       <c r="F206" s="7"/>
     </row>
     <row r="207" spans="1:18">
-      <c r="C207" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D207" s="7"/>
-      <c r="E207" s="7"/>
-      <c r="F207" s="7"/>
+      <c r="C207" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="D207" s="89">
+        <v>0.93059999999999998</v>
+      </c>
+      <c r="E207" s="89">
+        <v>0.86650000000000005</v>
+      </c>
+      <c r="F207" s="89">
+        <v>0.93059999999999998</v>
+      </c>
     </row>
     <row r="208" spans="1:18">
-      <c r="C208" s="91" t="s">
-        <v>118</v>
-      </c>
-      <c r="D208" s="89">
-        <v>0.93059999999999998</v>
-      </c>
-      <c r="E208" s="89">
-        <v>0.86650000000000005</v>
-      </c>
-      <c r="F208" s="89">
-        <v>0.93059999999999998</v>
-      </c>
+      <c r="C208" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D208" s="8"/>
+      <c r="E208" s="8"/>
+      <c r="F208" s="8"/>
     </row>
     <row r="209" spans="3:6">
       <c r="C209" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D209" s="8"/>
-      <c r="E209" s="8"/>
-      <c r="F209" s="8"/>
+        <v>120</v>
+      </c>
+      <c r="D209" s="2">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="E209" s="2">
+        <v>0.8367</v>
+      </c>
+      <c r="F209" s="2">
+        <v>0.88229999999999997</v>
+      </c>
     </row>
     <row r="210" spans="3:6">
-      <c r="C210" s="106" t="s">
-        <v>120</v>
+      <c r="C210" s="104" t="s">
+        <v>123</v>
       </c>
       <c r="D210" s="2">
-        <v>0.88619999999999999</v>
+        <v>0.29470000000000002</v>
       </c>
       <c r="E210" s="2">
-        <v>0.8367</v>
+        <v>0.14269999999999999</v>
       </c>
       <c r="F210" s="2">
-        <v>0.88229999999999997</v>
+        <v>0.27510000000000001</v>
       </c>
     </row>
     <row r="212" spans="3:6">
-      <c r="C212" s="105" t="s">
-        <v>123</v>
-      </c>
+      <c r="C212" s="41"/>
     </row>
     <row r="213" spans="3:6">
-      <c r="C213" s="105" t="s">
-        <v>124</v>
-      </c>
+      <c r="C213" s="41"/>
     </row>
     <row r="214" spans="3:6">
-      <c r="C214" s="105" t="s">
-        <v>125</v>
-      </c>
+      <c r="C214" s="41"/>
     </row>
     <row r="217" spans="3:6">
-      <c r="C217" s="104" t="s">
+      <c r="C217" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="D217" s="104" t="s">
+      <c r="D217" s="103" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="218" spans="3:6">
-      <c r="C218" s="104" t="s">
+      <c r="C218" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="D218" s="104" t="s">
+      <c r="D218" s="103" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="219" spans="3:6">
-      <c r="C219" s="104" t="s">
+      <c r="C219" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="D219" s="104" t="s">
+      <c r="D219" s="103" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add experiments for few-shots on chatgpt api
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777B1184-7830-DE49-A0E6-37743D5861EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB86840-F18A-8D42-9117-6A0DF04494E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="125">
   <si>
     <t>MIN</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>ChatGPT (two-staged)</t>
+  </si>
+  <si>
+    <t>ChatGPT (few-shots)</t>
   </si>
 </sst>
 </file>
@@ -958,7 +961,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1246,7 +1249,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1257,7 +1260,7 @@
   <dimension ref="A2:AE219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A192" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D211" sqref="D211"/>
+      <selection activeCell="H209" sqref="H209:H211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6167,7 +6170,7 @@
       </c>
     </row>
     <row r="210" spans="3:6">
-      <c r="C210" s="104" t="s">
+      <c r="C210" s="7" t="s">
         <v>123</v>
       </c>
       <c r="D210" s="2">
@@ -6179,6 +6182,14 @@
       <c r="F210" s="2">
         <v>0.27510000000000001</v>
       </c>
+    </row>
+    <row r="211" spans="3:6">
+      <c r="C211" s="104" t="s">
+        <v>124</v>
+      </c>
+      <c r="D211" s="8"/>
+      <c r="E211" s="8"/>
+      <c r="F211" s="8"/>
     </row>
     <row r="212" spans="3:6">
       <c r="C212" s="41"/>

</xml_diff>

<commit_message>
Update baseline: updade FSL with our outputs and ground truths
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F730C7-90EE-5A4E-8A83-4B94C544E27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C6AF56-8C63-714B-B1CD-AF9D69735517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="137">
   <si>
     <t>MIN</t>
   </si>
@@ -407,18 +407,6 @@
     <t>Edit</t>
   </si>
   <si>
-    <t>ChatGPT (two-staged)</t>
-  </si>
-  <si>
-    <t>ChatGPT (one-shot) highest</t>
-  </si>
-  <si>
-    <t>ChatGPT (one-shot) median</t>
-  </si>
-  <si>
-    <t>ChatGPT (one-shot) lowest</t>
-  </si>
-  <si>
     <t>Bard</t>
   </si>
   <si>
@@ -429,6 +417,39 @@
   </si>
   <si>
     <t>GPT-3.5</t>
+  </si>
+  <si>
+    <t>LLaMA (7B)</t>
+  </si>
+  <si>
+    <t>ChatGPT (zero-shot)</t>
+  </si>
+  <si>
+    <t>ChatGPT (one-shot) mean</t>
+  </si>
+  <si>
+    <t>max_input_len</t>
+  </si>
+  <si>
+    <t>truncated</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>learn with outputs from BART</t>
+  </si>
+  <si>
+    <t>learn with ground truth</t>
+  </si>
+  <si>
+    <t>ChatGPT (one-shot) max</t>
+  </si>
+  <si>
+    <t>ChatGPT (one-shot) min</t>
   </si>
 </sst>
 </file>
@@ -710,7 +731,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -959,6 +980,10 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1275,21 +1300,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="A2:AE219"/>
+  <dimension ref="A2:AE224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="G209" sqref="G209"/>
+    <sheetView tabSelected="1" topLeftCell="A198" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="0.1640625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="9.5" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" customWidth="1"/>
     <col min="12" max="12" width="9.33203125" customWidth="1"/>
@@ -6121,175 +6146,386 @@
         <v>16</v>
       </c>
       <c r="H203" s="105" t="s">
-        <v>128</v>
+        <v>124</v>
+      </c>
+      <c r="I203" s="105" t="s">
+        <v>129</v>
+      </c>
+      <c r="J203" s="105" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="204" spans="1:18">
       <c r="C204" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="D204" s="2">
+      <c r="D204" s="84">
         <v>0.98160000000000003</v>
       </c>
-      <c r="E204" s="2">
+      <c r="E204" s="84">
         <v>0.97489999999999999</v>
       </c>
-      <c r="F204" s="2">
+      <c r="F204" s="84">
         <v>0.98140000000000005</v>
       </c>
       <c r="H204" s="105">
         <v>168</v>
+      </c>
+      <c r="J204" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="205" spans="1:18">
       <c r="C205" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D205" s="2">
+      <c r="D205" s="84">
         <v>6.9500000000000006E-2</v>
       </c>
-      <c r="E205" s="2">
+      <c r="E205" s="84">
         <v>3.7199999999999997E-2</v>
       </c>
-      <c r="F205" s="2">
+      <c r="F205" s="84">
         <v>6.7599999999999993E-2</v>
       </c>
       <c r="H205" s="105">
         <v>168</v>
+      </c>
+      <c r="I205" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J205" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="206" spans="1:18">
       <c r="C206" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D206" s="2">
+      <c r="D206" s="84">
         <v>0.51849999999999996</v>
       </c>
-      <c r="E206" s="2">
+      <c r="E206" s="84">
         <v>0.47049999999999997</v>
       </c>
-      <c r="F206" s="2">
+      <c r="F206" s="84">
         <v>0.51790000000000003</v>
       </c>
       <c r="H206" s="105">
         <v>168</v>
+      </c>
+      <c r="I206" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J206" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="207" spans="1:18">
       <c r="C207" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D207" s="2">
-        <v>0.88619999999999999</v>
-      </c>
-      <c r="E207" s="2">
-        <v>0.8367</v>
-      </c>
-      <c r="F207" s="2">
-        <v>0.88229999999999997</v>
+      <c r="D207" s="84">
+        <v>0.88149999999999995</v>
+      </c>
+      <c r="E207" s="84">
+        <v>0.82679999999999998</v>
+      </c>
+      <c r="F207" s="84">
+        <v>0.87780000000000002</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H207" s="105">
         <v>168</v>
       </c>
+      <c r="I207" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J207" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="208" spans="1:18">
       <c r="C208" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D208" s="2">
-        <v>0.29470000000000002</v>
-      </c>
-      <c r="E208" s="2">
-        <v>0.14269999999999999</v>
-      </c>
-      <c r="F208" s="2">
-        <v>0.27510000000000001</v>
+        <v>127</v>
+      </c>
+      <c r="D208" s="84">
+        <v>0.34439999999999998</v>
+      </c>
+      <c r="E208" s="84">
+        <v>0.17019999999999999</v>
+      </c>
+      <c r="F208" s="84">
+        <v>0.32240000000000002</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="H208" s="105">
         <v>87</v>
       </c>
-    </row>
-    <row r="209" spans="3:6">
+      <c r="I208" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J208" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="209" spans="3:11">
       <c r="C209" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D209" s="84">
+        <v>0.42180000000000001</v>
+      </c>
+      <c r="E209" s="84">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="F209" s="84">
+        <v>0.39489999999999997</v>
+      </c>
+      <c r="G209" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H209" s="105">
+        <v>87</v>
+      </c>
+      <c r="I209" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J209" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K209" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="210" spans="3:11">
+      <c r="C210" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D210" s="84">
+        <v>0.4405</v>
+      </c>
+      <c r="E210" s="84">
+        <v>0.2492</v>
+      </c>
+      <c r="F210" s="84">
+        <v>0.41510000000000002</v>
+      </c>
+      <c r="G210" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H210" s="105">
+        <v>87</v>
+      </c>
+      <c r="I210" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J210" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K210" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="211" spans="3:11">
+      <c r="C211" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D211" s="84">
+        <v>0.43880000000000002</v>
+      </c>
+      <c r="E211" s="84">
+        <v>0.24110000000000001</v>
+      </c>
+      <c r="F211" s="84">
+        <v>0.41120000000000001</v>
+      </c>
+      <c r="G211" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H211" s="105">
+        <v>87</v>
+      </c>
+      <c r="I211" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J211" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K211" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="212" spans="3:11">
+      <c r="C212" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D212" s="84">
+        <v>0.42970000000000003</v>
+      </c>
+      <c r="E212" s="84">
+        <v>0.2427</v>
+      </c>
+      <c r="F212" s="84">
+        <v>0.40739999999999998</v>
+      </c>
+      <c r="G212" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H212" s="105">
+        <v>87</v>
+      </c>
+      <c r="I212" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J212" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K212" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="213" spans="3:11">
+      <c r="C213" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D213" s="84">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="E213" s="84">
+        <v>0.24729999999999999</v>
+      </c>
+      <c r="F213" s="84">
+        <v>0.41170000000000001</v>
+      </c>
+      <c r="G213" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H213" s="105">
+        <v>87</v>
+      </c>
+      <c r="I213" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J213" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K213" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="214" spans="3:11">
+      <c r="C214" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D214" s="84">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E214" s="84">
+        <v>0.25440000000000002</v>
+      </c>
+      <c r="F214" s="84">
+        <v>0.42159999999999997</v>
+      </c>
+      <c r="G214" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H214" s="105">
+        <v>87</v>
+      </c>
+      <c r="I214" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J214" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K214" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="215" spans="3:11">
+      <c r="C215" s="104" t="s">
+        <v>122</v>
+      </c>
+      <c r="D215" s="106"/>
+      <c r="E215" s="106"/>
+      <c r="F215" s="106"/>
+      <c r="H215" s="105"/>
+      <c r="I215" s="1">
+        <v>2048</v>
+      </c>
+      <c r="J215" s="1"/>
+    </row>
+    <row r="216" spans="3:11">
+      <c r="C216" s="104" t="s">
         <v>123</v>
       </c>
-      <c r="D209" s="8"/>
-      <c r="E209" s="8"/>
-      <c r="F209" s="8"/>
-    </row>
-    <row r="210" spans="3:6">
-      <c r="C210" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D210" s="8"/>
-      <c r="E210" s="8"/>
-      <c r="F210" s="8"/>
-    </row>
-    <row r="211" spans="3:6">
-      <c r="C211" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D211" s="8"/>
-      <c r="E211" s="8"/>
-      <c r="F211" s="8"/>
-    </row>
-    <row r="212" spans="3:6">
-      <c r="C212" s="104" t="s">
+      <c r="D216" s="106"/>
+      <c r="E216" s="106"/>
+      <c r="F216" s="106"/>
+      <c r="H216" s="105"/>
+      <c r="I216" s="1"/>
+      <c r="J216" s="1"/>
+    </row>
+    <row r="217" spans="3:11">
+      <c r="C217" s="104" t="s">
         <v>126</v>
       </c>
-      <c r="D212" s="8"/>
-      <c r="E212" s="8"/>
-      <c r="F212" s="8"/>
-    </row>
-    <row r="213" spans="3:6">
-      <c r="C213" s="104" t="s">
-        <v>127</v>
-      </c>
-      <c r="D213" s="8"/>
-      <c r="E213" s="8"/>
-      <c r="F213" s="8"/>
-    </row>
-    <row r="214" spans="3:6">
-      <c r="C214" s="91" t="s">
+      <c r="D217" s="106"/>
+      <c r="E217" s="106"/>
+      <c r="F217" s="106"/>
+      <c r="H217" s="105"/>
+      <c r="I217" s="1"/>
+      <c r="J217" s="1"/>
+    </row>
+    <row r="218" spans="3:11">
+      <c r="C218" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="D214" s="30">
-        <v>0.93059999999999998</v>
-      </c>
-      <c r="E214" s="30">
-        <v>0.86650000000000005</v>
-      </c>
-      <c r="F214" s="30">
-        <v>0.93059999999999998</v>
-      </c>
-    </row>
-    <row r="217" spans="3:6">
-      <c r="C217" s="103" t="s">
+      <c r="D218" s="107">
+        <v>0.91790000000000005</v>
+      </c>
+      <c r="E218" s="107">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="F218" s="107">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="H218" s="105">
+        <v>168</v>
+      </c>
+      <c r="I218" s="1">
+        <v>4096</v>
+      </c>
+      <c r="J218" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="222" spans="3:11">
+      <c r="C222" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="D217" s="103" t="s">
+      <c r="D222" s="103" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="218" spans="3:6">
-      <c r="C218" s="103" t="s">
+    <row r="223" spans="3:11">
+      <c r="C223" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="D218" s="103" t="s">
+      <c r="D223" s="103" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="219" spans="3:6">
-      <c r="C219" s="103" t="s">
+    <row r="224" spans="3:11">
+      <c r="C224" s="103" t="s">
         <v>114</v>
       </c>
-      <c r="D219" s="103" t="s">
+      <c r="D224" s="103" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the current todo and baselines
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB79AED-E54E-C74B-A059-044C016CB8D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9182E8E8-D9E5-0B40-A648-0529234ABD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="136">
   <si>
     <t>MIN</t>
   </si>
@@ -410,9 +410,6 @@
     <t>#instances</t>
   </si>
   <si>
-    <t>GPT-3.5</t>
-  </si>
-  <si>
     <t>ChatGPT (zero-shot)</t>
   </si>
   <si>
@@ -443,16 +440,13 @@
     <t>ChatGPT (one-shot) min</t>
   </si>
   <si>
-    <t>3 or 5</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shots) max</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shots) mean</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shots) min</t>
+    <t>GPT-4 (few-shot-3) max</t>
+  </si>
+  <si>
+    <t>GPT-4 (few-shot-3) mean</t>
+  </si>
+  <si>
+    <t>GPT-4 (few-shot-3) min</t>
   </si>
 </sst>
 </file>
@@ -1307,7 +1301,7 @@
   <dimension ref="A2:AE231"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A201" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="D219" sqref="D219"/>
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6149,14 +6143,14 @@
       <c r="F203" s="34" t="s">
         <v>16</v>
       </c>
+      <c r="G203" s="105" t="s">
+        <v>122</v>
+      </c>
       <c r="H203" s="105" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="I203" s="105" t="s">
         <v>126</v>
-      </c>
-      <c r="J203" s="105" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="204" spans="1:18">
@@ -6172,11 +6166,11 @@
       <c r="F204" s="84">
         <v>0.98140000000000005</v>
       </c>
-      <c r="H204" s="105">
+      <c r="G204" s="105">
         <v>168</v>
       </c>
-      <c r="J204" s="1" t="s">
-        <v>128</v>
+      <c r="I204" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="205" spans="1:18">
@@ -6192,14 +6186,14 @@
       <c r="F205" s="84">
         <v>6.7599999999999993E-2</v>
       </c>
-      <c r="H205" s="105">
+      <c r="G205" s="105">
         <v>168</v>
       </c>
-      <c r="I205" s="1">
+      <c r="H205" s="1">
         <v>4096</v>
       </c>
-      <c r="J205" s="1" t="s">
-        <v>129</v>
+      <c r="I205" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="206" spans="1:18">
@@ -6215,14 +6209,14 @@
       <c r="F206" s="84">
         <v>0.51790000000000003</v>
       </c>
-      <c r="H206" s="105">
+      <c r="G206" s="105">
         <v>168</v>
       </c>
-      <c r="I206" s="1">
+      <c r="H206" s="1">
         <v>4096</v>
       </c>
-      <c r="J206" s="1" t="s">
-        <v>129</v>
+      <c r="I206" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="207" spans="1:18">
@@ -6238,316 +6232,297 @@
       <c r="F207" s="84">
         <v>0.87780000000000002</v>
       </c>
-      <c r="G207" s="1" t="s">
+      <c r="G207" s="105">
+        <v>168</v>
+      </c>
+      <c r="H207" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I207" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="208" spans="1:18">
+      <c r="C208" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="D208" s="107">
+        <v>0.91790000000000005</v>
+      </c>
+      <c r="E208" s="107">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="F208" s="107">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="G208" s="105">
+        <v>168</v>
+      </c>
+      <c r="H208" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I208" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="209" spans="3:10">
+      <c r="C209" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="H207" s="105">
-        <v>168</v>
-      </c>
-      <c r="I207" s="1">
+      <c r="D209" s="84">
+        <v>0.34439999999999998</v>
+      </c>
+      <c r="E209" s="84">
+        <v>0.17019999999999999</v>
+      </c>
+      <c r="F209" s="84">
+        <v>0.32240000000000002</v>
+      </c>
+      <c r="G209" s="105">
+        <v>87</v>
+      </c>
+      <c r="H209" s="1">
         <v>4096</v>
       </c>
-      <c r="J207" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="208" spans="1:18">
-      <c r="C208" s="7" t="s">
+      <c r="I209" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="210" spans="3:10">
+      <c r="C210" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D210" s="84">
+        <v>0.42180000000000001</v>
+      </c>
+      <c r="E210" s="84">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="F210" s="84">
+        <v>0.39489999999999997</v>
+      </c>
+      <c r="G210" s="105">
+        <v>87</v>
+      </c>
+      <c r="H210" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I210" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J210" s="41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="211" spans="3:10">
+      <c r="C211" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D208" s="84">
-        <v>0.34439999999999998</v>
-      </c>
-      <c r="E208" s="84">
-        <v>0.17019999999999999</v>
-      </c>
-      <c r="F208" s="84">
-        <v>0.32240000000000002</v>
-      </c>
-      <c r="G208" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H208" s="105">
+      <c r="D211" s="84">
+        <v>0.4405</v>
+      </c>
+      <c r="E211" s="84">
+        <v>0.2492</v>
+      </c>
+      <c r="F211" s="84">
+        <v>0.41510000000000002</v>
+      </c>
+      <c r="G211" s="105">
         <v>87</v>
       </c>
-      <c r="I208" s="1">
+      <c r="H211" s="1">
         <v>4096</v>
       </c>
-      <c r="J208" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="209" spans="3:11">
-      <c r="C209" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D209" s="84">
-        <v>0.42180000000000001</v>
-      </c>
-      <c r="E209" s="84">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="F209" s="84">
-        <v>0.39489999999999997</v>
-      </c>
-      <c r="G209" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H209" s="105">
-        <v>87</v>
-      </c>
-      <c r="I209" s="1">
-        <v>4096</v>
-      </c>
-      <c r="J209" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K209" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="210" spans="3:11">
-      <c r="C210" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D210" s="84">
-        <v>0.4405</v>
-      </c>
-      <c r="E210" s="84">
-        <v>0.2492</v>
-      </c>
-      <c r="F210" s="84">
-        <v>0.41510000000000002</v>
-      </c>
-      <c r="G210" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H210" s="105">
-        <v>87</v>
-      </c>
-      <c r="I210" s="1">
-        <v>4096</v>
-      </c>
-      <c r="J210" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K210" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="211" spans="3:11">
-      <c r="C211" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D211" s="84">
-        <v>0.43880000000000002</v>
-      </c>
-      <c r="E211" s="84">
-        <v>0.24110000000000001</v>
-      </c>
-      <c r="F211" s="84">
-        <v>0.41120000000000001</v>
-      </c>
-      <c r="G211" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H211" s="105">
-        <v>87</v>
-      </c>
-      <c r="I211" s="1">
-        <v>4096</v>
-      </c>
-      <c r="J211" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K211" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="212" spans="3:11">
+      <c r="I211" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J211" s="41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="212" spans="3:10">
       <c r="C212" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D212" s="84">
+        <v>0.43880000000000002</v>
+      </c>
+      <c r="E212" s="84">
+        <v>0.24110000000000001</v>
+      </c>
+      <c r="F212" s="84">
+        <v>0.41120000000000001</v>
+      </c>
+      <c r="G212" s="105">
+        <v>87</v>
+      </c>
+      <c r="H212" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I212" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J212" s="41" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="213" spans="3:10">
+      <c r="C213" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D213" s="84">
         <v>0.42970000000000003</v>
       </c>
-      <c r="E212" s="84">
+      <c r="E213" s="84">
         <v>0.2427</v>
       </c>
-      <c r="F212" s="84">
+      <c r="F213" s="84">
         <v>0.40739999999999998</v>
       </c>
-      <c r="G212" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H212" s="105">
+      <c r="G213" s="105">
         <v>87</v>
       </c>
-      <c r="I212" s="1">
+      <c r="H213" s="1">
         <v>4096</v>
       </c>
-      <c r="J212" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K212" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="213" spans="3:11">
-      <c r="C213" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D213" s="84">
+      <c r="I213" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J213" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="214" spans="3:10">
+      <c r="C214" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D214" s="84">
         <v>0.44040000000000001</v>
       </c>
-      <c r="E213" s="84">
+      <c r="E214" s="84">
         <v>0.24729999999999999</v>
       </c>
-      <c r="F213" s="84">
+      <c r="F214" s="84">
         <v>0.41170000000000001</v>
       </c>
-      <c r="G213" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H213" s="105">
+      <c r="G214" s="105">
         <v>87</v>
       </c>
-      <c r="I213" s="1">
+      <c r="H214" s="1">
         <v>4096</v>
       </c>
-      <c r="J213" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K213" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="214" spans="3:11">
-      <c r="C214" s="7" t="s">
+      <c r="I214" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J214" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="215" spans="3:10">
+      <c r="C215" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D215" s="84">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E215" s="84">
+        <v>0.25440000000000002</v>
+      </c>
+      <c r="F215" s="84">
+        <v>0.42159999999999997</v>
+      </c>
+      <c r="G215" s="105">
+        <v>87</v>
+      </c>
+      <c r="H215" s="1">
+        <v>4096</v>
+      </c>
+      <c r="I215" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J215" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="216" spans="3:10">
+      <c r="C216" s="104" t="s">
         <v>133</v>
-      </c>
-      <c r="D214" s="84">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="E214" s="84">
-        <v>0.25440000000000002</v>
-      </c>
-      <c r="F214" s="84">
-        <v>0.42159999999999997</v>
-      </c>
-      <c r="G214" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="H214" s="105">
-        <v>87</v>
-      </c>
-      <c r="I214" s="1">
-        <v>4096</v>
-      </c>
-      <c r="J214" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K214" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="215" spans="3:11">
-      <c r="C215" s="104" t="s">
-        <v>135</v>
-      </c>
-      <c r="D215" s="106"/>
-      <c r="E215" s="106"/>
-      <c r="F215" s="106"/>
-      <c r="H215" s="105">
-        <v>87</v>
-      </c>
-      <c r="I215" s="1"/>
-      <c r="J215" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K215" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="216" spans="3:11">
-      <c r="C216" s="104" t="s">
-        <v>136</v>
       </c>
       <c r="D216" s="106"/>
       <c r="E216" s="106"/>
       <c r="F216" s="106"/>
-      <c r="H216" s="105">
+      <c r="G216" s="105">
         <v>87</v>
       </c>
-      <c r="I216" s="1"/>
-      <c r="J216" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K216" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="217" spans="3:11">
+      <c r="H216" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I216" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J216" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="217" spans="3:10">
       <c r="C217" s="104" t="s">
-        <v>137</v>
-      </c>
-      <c r="D217" s="8"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="H217" s="105">
+        <v>134</v>
+      </c>
+      <c r="D217" s="106"/>
+      <c r="E217" s="106"/>
+      <c r="F217" s="106"/>
+      <c r="G217" s="105">
         <v>87</v>
       </c>
-      <c r="J217" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="K217" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="218" spans="3:11">
-      <c r="C218" s="91" t="s">
-        <v>118</v>
-      </c>
-      <c r="D218" s="107">
-        <v>0.91790000000000005</v>
-      </c>
-      <c r="E218" s="107">
-        <v>0.84140000000000004</v>
-      </c>
-      <c r="F218" s="107">
-        <v>0.91769999999999996</v>
-      </c>
-      <c r="H218" s="105">
-        <v>168</v>
-      </c>
-      <c r="I218" s="1">
-        <v>4096</v>
-      </c>
-      <c r="J218" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="219" spans="3:11">
+      <c r="H217" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I217" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J217" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="218" spans="3:10">
+      <c r="C218" s="104" t="s">
+        <v>135</v>
+      </c>
+      <c r="D218" s="8"/>
+      <c r="E218" s="8"/>
+      <c r="F218" s="8"/>
+      <c r="G218" s="105">
+        <v>87</v>
+      </c>
+      <c r="H218" s="1">
+        <v>8192</v>
+      </c>
+      <c r="I218" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J218" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="219" spans="3:10">
       <c r="C219" s="91" t="s">
         <v>118</v>
       </c>
       <c r="D219" s="107"/>
       <c r="E219" s="107"/>
       <c r="F219" s="107"/>
-      <c r="H219" s="105">
+      <c r="G219" s="105">
         <v>87</v>
       </c>
-      <c r="I219" s="1">
+      <c r="H219" s="1">
         <v>4096</v>
       </c>
-      <c r="J219" s="1" t="s">
-        <v>128</v>
+      <c r="I219" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="228" spans="3:6">
-      <c r="F228" s="108" t="s">
-        <v>134</v>
-      </c>
+      <c r="F228" s="108"/>
     </row>
     <row r="229" spans="3:6">
       <c r="C229" s="103" t="s">

</xml_diff>

<commit_message>
Update experiment results (BART) in restricted mode
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9182E8E8-D9E5-0B40-A648-0529234ABD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF43BD1-C55B-154E-8ADE-E06FD834CEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="136">
   <si>
     <t>MIN</t>
   </si>
@@ -545,7 +545,7 @@
       <name val="Times Nw"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +561,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,7 +734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -984,6 +990,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1300,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="I224" sqref="I224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6265,7 +6283,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="209" spans="3:10">
+    <row r="209" spans="3:11">
       <c r="C209" s="7" t="s">
         <v>123</v>
       </c>
@@ -6288,85 +6306,88 @@
         <v>127</v>
       </c>
     </row>
-    <row r="210" spans="3:10">
-      <c r="C210" s="7" t="s">
+    <row r="210" spans="3:11">
+      <c r="C210" s="109" t="s">
         <v>131</v>
       </c>
-      <c r="D210" s="84">
+      <c r="D210" s="110">
         <v>0.42180000000000001</v>
       </c>
-      <c r="E210" s="84">
+      <c r="E210" s="110">
         <v>0.22700000000000001</v>
       </c>
-      <c r="F210" s="84">
+      <c r="F210" s="110">
         <v>0.39489999999999997</v>
       </c>
-      <c r="G210" s="105">
+      <c r="G210" s="111">
         <v>87</v>
       </c>
-      <c r="H210" s="1">
+      <c r="H210" s="112">
         <v>4096</v>
       </c>
-      <c r="I210" s="1" t="s">
+      <c r="I210" s="112" t="s">
         <v>127</v>
       </c>
-      <c r="J210" s="41" t="s">
+      <c r="J210" s="113" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="211" spans="3:10">
-      <c r="C211" s="7" t="s">
+      <c r="K210" s="114"/>
+    </row>
+    <row r="211" spans="3:11">
+      <c r="C211" s="109" t="s">
         <v>124</v>
       </c>
-      <c r="D211" s="84">
+      <c r="D211" s="110">
         <v>0.4405</v>
       </c>
-      <c r="E211" s="84">
+      <c r="E211" s="110">
         <v>0.2492</v>
       </c>
-      <c r="F211" s="84">
+      <c r="F211" s="110">
         <v>0.41510000000000002</v>
       </c>
-      <c r="G211" s="105">
+      <c r="G211" s="111">
         <v>87</v>
       </c>
-      <c r="H211" s="1">
+      <c r="H211" s="112">
         <v>4096</v>
       </c>
-      <c r="I211" s="1" t="s">
+      <c r="I211" s="112" t="s">
         <v>127</v>
       </c>
-      <c r="J211" s="41" t="s">
+      <c r="J211" s="113" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="212" spans="3:10">
-      <c r="C212" s="7" t="s">
+      <c r="K211" s="114"/>
+    </row>
+    <row r="212" spans="3:11">
+      <c r="C212" s="109" t="s">
         <v>132</v>
       </c>
-      <c r="D212" s="84">
+      <c r="D212" s="110">
         <v>0.43880000000000002</v>
       </c>
-      <c r="E212" s="84">
+      <c r="E212" s="110">
         <v>0.24110000000000001</v>
       </c>
-      <c r="F212" s="84">
+      <c r="F212" s="110">
         <v>0.41120000000000001</v>
       </c>
-      <c r="G212" s="105">
+      <c r="G212" s="111">
         <v>87</v>
       </c>
-      <c r="H212" s="1">
+      <c r="H212" s="112">
         <v>4096</v>
       </c>
-      <c r="I212" s="1" t="s">
+      <c r="I212" s="112" t="s">
         <v>127</v>
       </c>
-      <c r="J212" s="41" t="s">
+      <c r="J212" s="113" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="213" spans="3:10">
+      <c r="K212" s="114"/>
+    </row>
+    <row r="213" spans="3:11">
       <c r="C213" s="7" t="s">
         <v>131</v>
       </c>
@@ -6392,7 +6413,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="214" spans="3:10">
+    <row r="214" spans="3:11">
       <c r="C214" s="7" t="s">
         <v>124</v>
       </c>
@@ -6418,7 +6439,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="215" spans="3:10">
+    <row r="215" spans="3:11">
       <c r="C215" s="7" t="s">
         <v>132</v>
       </c>
@@ -6444,7 +6465,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="216" spans="3:10">
+    <row r="216" spans="3:11">
       <c r="C216" s="104" t="s">
         <v>133</v>
       </c>
@@ -6464,7 +6485,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="217" spans="3:10">
+    <row r="217" spans="3:11">
       <c r="C217" s="104" t="s">
         <v>134</v>
       </c>
@@ -6484,7 +6505,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="218" spans="3:10">
+    <row r="218" spans="3:11">
       <c r="C218" s="104" t="s">
         <v>135</v>
       </c>
@@ -6504,13 +6525,19 @@
         <v>130</v>
       </c>
     </row>
-    <row r="219" spans="3:10">
+    <row r="219" spans="3:11">
       <c r="C219" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="D219" s="107"/>
-      <c r="E219" s="107"/>
-      <c r="F219" s="107"/>
+      <c r="D219" s="107">
+        <v>0.8468</v>
+      </c>
+      <c r="E219" s="107">
+        <v>0.79490000000000005</v>
+      </c>
+      <c r="F219" s="107">
+        <v>0.84389999999999998</v>
+      </c>
       <c r="G219" s="105">
         <v>87</v>
       </c>
@@ -6519,6 +6546,9 @@
       </c>
       <c r="I219" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="J219" s="41" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="228" spans="3:6">

</xml_diff>

<commit_message>
Update baseline: inputs for decoding
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381455A0-8340-C140-B287-817391D63BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DF5C9-AFA1-FE46-9E4A-6FE11B5CA21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="139">
   <si>
     <t>MIN</t>
   </si>
@@ -398,9 +398,6 @@
     <t>BART (two-staged)</t>
   </si>
   <si>
-    <t>ChatGPT (decoder)</t>
-  </si>
-  <si>
     <t>Completion</t>
   </si>
   <si>
@@ -425,15 +422,6 @@
     <t>ChatGPT (one-shot) min</t>
   </si>
   <si>
-    <t>GPT-4 (few-shot-3) max</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shot-3) mean</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shot-3) min</t>
-  </si>
-  <si>
     <t>GPT-3.5 (zero-shot)</t>
   </si>
   <si>
@@ -446,34 +434,28 @@
     <t>GPT-3.5 (one-shot) min</t>
   </si>
   <si>
-    <t>GPT-4 (few-shot-5) max</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shot-5) mean</t>
-  </si>
-  <si>
-    <t>GPT-4 (few-shot-5) min</t>
-  </si>
-  <si>
     <t>GPT-4 (zero-shot)</t>
   </si>
   <si>
-    <t>GPT-4 (one-shot) max</t>
-  </si>
-  <si>
-    <t>GPT-4 (one-shot) mean</t>
-  </si>
-  <si>
-    <t>GPT-4 (one-shot) min</t>
-  </si>
-  <si>
-    <t>LLaMA (7B) (zeroshot)</t>
-  </si>
-  <si>
-    <t>LLaMA (7B) oneshot</t>
-  </si>
-  <si>
-    <t>max input length: 3856</t>
+    <t>GPT-3.5 (decoder)</t>
+  </si>
+  <si>
+    <t>Vicuna (13B) (zero-shot)</t>
+  </si>
+  <si>
+    <t>GPT-4 (decoder)</t>
+  </si>
+  <si>
+    <t>LLaMA (7B) (decoder)</t>
+  </si>
+  <si>
+    <t>Vicuna (13B) (decoder)</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>For Decoding (paragraph-level)</t>
   </si>
 </sst>
 </file>
@@ -767,7 +749,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1033,6 +1015,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1350,15 +1335,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C231" sqref="C231:G231"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G230" sqref="G230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="1.5" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.83203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="8" max="9" width="12.83203125" customWidth="1"/>
@@ -1897,10 +1882,10 @@
         <v>0.91</v>
       </c>
       <c r="Y22" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z22" t="s">
         <v>120</v>
-      </c>
-      <c r="Z22" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="23" spans="2:31">
@@ -6199,10 +6184,10 @@
         <v>16</v>
       </c>
       <c r="G203" s="89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H203" s="89" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I203" s="1"/>
     </row>
@@ -6227,37 +6212,25 @@
     </row>
     <row r="205" spans="1:18">
       <c r="C205" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D205" s="84">
-        <v>6.9500000000000006E-2</v>
-      </c>
-      <c r="E205" s="84">
-        <v>3.7199999999999997E-2</v>
-      </c>
-      <c r="F205" s="84">
-        <v>6.7599999999999993E-2</v>
-      </c>
-      <c r="G205" s="2">
-        <v>168</v>
-      </c>
-      <c r="H205" s="2">
-        <v>4096</v>
+        <v>115</v>
+      </c>
+      <c r="G205" s="1">
+        <v>87</v>
       </c>
       <c r="I205" s="1"/>
     </row>
     <row r="206" spans="1:18">
       <c r="C206" s="7" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D206" s="84">
-        <v>0.51849999999999996</v>
+        <v>6.9500000000000006E-2</v>
       </c>
       <c r="E206" s="84">
-        <v>0.47049999999999997</v>
+        <v>3.7199999999999997E-2</v>
       </c>
       <c r="F206" s="84">
-        <v>0.51790000000000003</v>
+        <v>6.7599999999999993E-2</v>
       </c>
       <c r="G206" s="2">
         <v>168</v>
@@ -6269,16 +6242,16 @@
     </row>
     <row r="207" spans="1:18">
       <c r="C207" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D207" s="84">
-        <v>0.88149999999999995</v>
+        <v>0.51849999999999996</v>
       </c>
       <c r="E207" s="84">
-        <v>0.82679999999999998</v>
+        <v>0.47049999999999997</v>
       </c>
       <c r="F207" s="84">
-        <v>0.87780000000000002</v>
+        <v>0.51790000000000003</v>
       </c>
       <c r="G207" s="2">
         <v>168</v>
@@ -6304,63 +6277,55 @@
       <c r="G208" s="2">
         <v>168</v>
       </c>
-      <c r="H208" s="2"/>
       <c r="I208" s="1"/>
+      <c r="P208" s="2"/>
     </row>
     <row r="209" spans="3:9">
       <c r="C209" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D209" s="84">
-        <v>0.34439999999999998</v>
+        <v>0.88149999999999995</v>
       </c>
       <c r="E209" s="84">
-        <v>0.17019999999999999</v>
+        <v>0.82679999999999998</v>
       </c>
       <c r="F209" s="84">
-        <v>0.32240000000000002</v>
+        <v>0.87780000000000002</v>
       </c>
       <c r="G209" s="2">
-        <v>87</v>
+        <v>168</v>
       </c>
       <c r="H209" s="2">
         <v>4096</v>
       </c>
-      <c r="I209" s="1"/>
     </row>
     <row r="210" spans="3:9">
       <c r="C210" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="D210" s="84">
-        <v>0.42970000000000003</v>
-      </c>
-      <c r="E210" s="84">
-        <v>0.2427</v>
-      </c>
-      <c r="F210" s="84">
-        <v>0.40739999999999998</v>
-      </c>
+      <c r="D210" s="84"/>
+      <c r="E210" s="84"/>
+      <c r="F210" s="84"/>
       <c r="G210" s="2">
         <v>87</v>
       </c>
       <c r="H210" s="2">
         <v>4096</v>
       </c>
-      <c r="I210" s="41"/>
     </row>
     <row r="211" spans="3:9">
       <c r="C211" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D211" s="84">
-        <v>0.44040000000000001</v>
+        <v>0.34439999999999998</v>
       </c>
       <c r="E211" s="84">
-        <v>0.24729999999999999</v>
+        <v>0.17019999999999999</v>
       </c>
       <c r="F211" s="84">
-        <v>0.41170000000000001</v>
+        <v>0.32240000000000002</v>
       </c>
       <c r="G211" s="2">
         <v>87</v>
@@ -6368,20 +6333,20 @@
       <c r="H211" s="2">
         <v>4096</v>
       </c>
-      <c r="I211" s="41"/>
+      <c r="I211" s="1"/>
     </row>
     <row r="212" spans="3:9">
       <c r="C212" s="7" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D212" s="84">
-        <v>0.44700000000000001</v>
+        <v>0.42970000000000003</v>
       </c>
       <c r="E212" s="84">
-        <v>0.25440000000000002</v>
+        <v>0.2427</v>
       </c>
       <c r="F212" s="84">
-        <v>0.42159999999999997</v>
+        <v>0.40739999999999998</v>
       </c>
       <c r="G212" s="2">
         <v>87</v>
@@ -6393,37 +6358,49 @@
     </row>
     <row r="213" spans="3:9">
       <c r="C213" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D213" s="110"/>
-      <c r="E213" s="110"/>
-      <c r="F213" s="110"/>
+        <v>129</v>
+      </c>
+      <c r="D213" s="84">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="E213" s="84">
+        <v>0.24729999999999999</v>
+      </c>
+      <c r="F213" s="84">
+        <v>0.41170000000000001</v>
+      </c>
       <c r="G213" s="2">
         <v>87</v>
       </c>
       <c r="H213" s="2">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="I213" s="41"/>
     </row>
     <row r="214" spans="3:9">
       <c r="C214" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D214" s="110"/>
-      <c r="E214" s="110"/>
-      <c r="F214" s="110"/>
+        <v>130</v>
+      </c>
+      <c r="D214" s="84">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="E214" s="84">
+        <v>0.25440000000000002</v>
+      </c>
+      <c r="F214" s="84">
+        <v>0.42159999999999997</v>
+      </c>
       <c r="G214" s="2">
         <v>87</v>
       </c>
       <c r="H214" s="2">
-        <v>8192</v>
+        <v>4096</v>
       </c>
       <c r="I214" s="41"/>
     </row>
     <row r="215" spans="3:9">
       <c r="C215" s="7" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D215" s="110"/>
       <c r="E215" s="110"/>
@@ -6434,56 +6411,45 @@
       <c r="H215" s="2">
         <v>8192</v>
       </c>
-      <c r="I215" s="41"/>
     </row>
     <row r="216" spans="3:9">
       <c r="C216" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D216" s="8"/>
-      <c r="E216" s="8"/>
-      <c r="F216" s="8"/>
-      <c r="G216" s="2">
-        <v>87</v>
-      </c>
-      <c r="H216" s="2">
-        <v>8192</v>
-      </c>
-      <c r="I216" s="41"/>
+        <v>134</v>
+      </c>
     </row>
     <row r="217" spans="3:9">
-      <c r="C217" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D217" s="110"/>
-      <c r="E217" s="110"/>
-      <c r="F217" s="110"/>
+      <c r="C217" s="113" t="s">
+        <v>135</v>
+      </c>
+      <c r="D217" s="84"/>
+      <c r="E217" s="84"/>
+      <c r="F217" s="84"/>
       <c r="G217" s="2">
         <v>87</v>
       </c>
       <c r="H217" s="2">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="I217" s="41"/>
     </row>
     <row r="218" spans="3:9">
-      <c r="C218" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D218" s="110"/>
-      <c r="E218" s="110"/>
-      <c r="F218" s="110"/>
+      <c r="C218" s="113" t="s">
+        <v>136</v>
+      </c>
+      <c r="D218" s="8"/>
+      <c r="E218" s="8"/>
+      <c r="F218" s="8"/>
       <c r="G218" s="2">
         <v>87</v>
       </c>
-      <c r="H218" s="2">
-        <v>8192</v>
+      <c r="H218" s="114">
+        <v>2048</v>
       </c>
       <c r="I218" s="41"/>
     </row>
     <row r="219" spans="3:9">
-      <c r="C219" s="7" t="s">
-        <v>130</v>
+      <c r="C219" s="113" t="s">
+        <v>133</v>
       </c>
       <c r="D219" s="8"/>
       <c r="E219" s="8"/>
@@ -6491,104 +6457,103 @@
       <c r="G219" s="2">
         <v>87</v>
       </c>
-      <c r="H219" s="2">
-        <v>8192</v>
+      <c r="H219" s="114">
+        <v>2048</v>
       </c>
       <c r="I219" s="41"/>
     </row>
     <row r="220" spans="3:9">
-      <c r="C220" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D220" s="110"/>
-      <c r="E220" s="110"/>
-      <c r="F220" s="110"/>
-      <c r="G220" s="2">
+      <c r="C220" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="D220" s="103">
+        <v>0.8468</v>
+      </c>
+      <c r="E220" s="103">
+        <v>0.79490000000000005</v>
+      </c>
+      <c r="F220" s="103">
+        <v>0.84389999999999998</v>
+      </c>
+      <c r="G220" s="89">
         <v>87</v>
       </c>
-      <c r="H220" s="2">
-        <v>8192</v>
-      </c>
+      <c r="H220" s="89">
+        <v>4096</v>
+      </c>
+      <c r="I220" s="41"/>
     </row>
     <row r="221" spans="3:9">
-      <c r="C221" s="7" t="s">
-        <v>136</v>
-      </c>
+      <c r="C221" s="7"/>
       <c r="D221" s="110"/>
       <c r="E221" s="110"/>
       <c r="F221" s="110"/>
-      <c r="G221" s="2">
-        <v>87</v>
-      </c>
-      <c r="H221" s="2">
-        <v>8192</v>
-      </c>
+      <c r="G221" s="2"/>
+      <c r="H221" s="2"/>
+      <c r="I221" s="41"/>
     </row>
     <row r="222" spans="3:9">
-      <c r="C222" s="7" t="s">
+      <c r="C222" s="7"/>
+      <c r="D222" s="110"/>
+      <c r="E222" s="110"/>
+      <c r="F222" s="110"/>
+      <c r="G222" s="2"/>
+      <c r="H222" s="2"/>
+    </row>
+    <row r="223" spans="3:9">
+      <c r="C223" s="7"/>
+      <c r="D223" s="8"/>
+      <c r="E223" s="8"/>
+      <c r="F223" s="8"/>
+      <c r="G223" s="2"/>
+      <c r="H223" s="2"/>
+    </row>
+    <row r="226" spans="3:10">
+      <c r="C226" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E226" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F226" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G226" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="227" spans="3:10">
+      <c r="C227" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D222" s="8"/>
-      <c r="E222" s="8"/>
-      <c r="F222" s="8"/>
-      <c r="G222" s="2">
-        <v>87</v>
-      </c>
-      <c r="H222" s="2">
-        <v>8192</v>
-      </c>
-    </row>
-    <row r="223" spans="3:9">
-      <c r="C223" s="113" t="s">
-        <v>142</v>
-      </c>
-      <c r="D223" s="84">
-        <v>0.10340000000000001</v>
-      </c>
-      <c r="E223" s="84">
-        <v>1.95E-2</v>
-      </c>
-      <c r="F223" s="84">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="G223" s="2">
-        <v>87</v>
-      </c>
-      <c r="H223" s="2">
-        <v>2048</v>
-      </c>
-      <c r="I223" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="224" spans="3:9">
-      <c r="C224" s="113" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="231" spans="3:10">
-      <c r="C231" s="91" t="s">
-        <v>118</v>
-      </c>
-      <c r="D231" s="103">
-        <v>0.8468</v>
-      </c>
-      <c r="E231" s="103">
-        <v>0.79490000000000005</v>
-      </c>
-      <c r="F231" s="103">
-        <v>0.84389999999999998</v>
-      </c>
-      <c r="G231" s="89">
-        <v>87</v>
-      </c>
-      <c r="H231" s="89">
-        <v>4096</v>
-      </c>
+      <c r="D227" s="4">
+        <v>162</v>
+      </c>
+      <c r="E227" s="4">
+        <v>253</v>
+      </c>
+      <c r="F227" s="4">
+        <v>187.7116</v>
+      </c>
+      <c r="G227" s="37">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="228" spans="3:10">
+      <c r="C228" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D228" s="4"/>
+      <c r="E228" s="4"/>
+      <c r="F228" s="4"/>
+      <c r="G228" s="37"/>
     </row>
     <row r="234" spans="3:10">
       <c r="C234" s="105" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D234" s="106">
         <v>0.42180000000000001</v>
@@ -6606,13 +6571,13 @@
         <v>4096</v>
       </c>
       <c r="I234" s="108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J234" s="109"/>
     </row>
     <row r="235" spans="3:10">
       <c r="C235" s="105" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D235" s="106">
         <v>0.4405</v>
@@ -6630,13 +6595,13 @@
         <v>4096</v>
       </c>
       <c r="I235" s="108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J235" s="109"/>
     </row>
     <row r="236" spans="3:10">
       <c r="C236" s="105" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D236" s="106">
         <v>0.43880000000000002</v>
@@ -6654,7 +6619,7 @@
         <v>4096</v>
       </c>
       <c r="I236" s="108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J236" s="109"/>
     </row>

</xml_diff>

<commit_message>
Migrate outputs to ./generation
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D95DF5C9-AFA1-FE46-9E4A-6FE11B5CA21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC151094-87E2-B44D-BD6D-1FAD43BCB676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -1335,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G230" sqref="G230"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J218" sqref="J218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Add #sampling for finetuning Vicuna
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC151094-87E2-B44D-BD6D-1FAD43BCB676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056CBB3A-597D-B64A-A368-A03A5DC02DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="142">
   <si>
     <t>MIN</t>
   </si>
@@ -456,6 +456,15 @@
   </si>
   <si>
     <t>For Decoding (paragraph-level)</t>
+  </si>
+  <si>
+    <t># train data for finetuning with Vicuna+LoRA</t>
+  </si>
+  <si>
+    <t>2000+2000</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1025,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1336,7 +1345,7 @@
   <dimension ref="A2:AE241"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A201" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J218" sqref="J218"/>
+      <selection activeCell="K230" sqref="K230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6442,7 +6451,7 @@
       <c r="G218" s="2">
         <v>87</v>
       </c>
-      <c r="H218" s="114">
+      <c r="H218" s="2">
         <v>2048</v>
       </c>
       <c r="I218" s="41"/>
@@ -6457,7 +6466,7 @@
       <c r="G219" s="2">
         <v>87</v>
       </c>
-      <c r="H219" s="114">
+      <c r="H219" s="2">
         <v>2048</v>
       </c>
       <c r="I219" s="41"/>
@@ -6508,7 +6517,7 @@
       <c r="G223" s="2"/>
       <c r="H223" s="2"/>
     </row>
-    <row r="226" spans="3:10">
+    <row r="226" spans="3:11">
       <c r="C226" s="4" t="s">
         <v>138</v>
       </c>
@@ -6525,7 +6534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="227" spans="3:10">
+    <row r="227" spans="3:11">
       <c r="C227" s="4" t="s">
         <v>137</v>
       </c>
@@ -6542,7 +6551,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="228" spans="3:10">
+    <row r="228" spans="3:11">
       <c r="C228" s="4" t="s">
         <v>25</v>
       </c>
@@ -6551,7 +6560,20 @@
       <c r="F228" s="4"/>
       <c r="G228" s="37"/>
     </row>
-    <row r="234" spans="3:10">
+    <row r="229" spans="3:11">
+      <c r="I229" s="114" t="s">
+        <v>139</v>
+      </c>
+      <c r="K229" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="230" spans="3:11">
+      <c r="K230" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="234" spans="3:11">
       <c r="C234" s="105" t="s">
         <v>125</v>
       </c>
@@ -6575,7 +6597,7 @@
       </c>
       <c r="J234" s="109"/>
     </row>
-    <row r="235" spans="3:10">
+    <row r="235" spans="3:11">
       <c r="C235" s="105" t="s">
         <v>122</v>
       </c>
@@ -6599,7 +6621,7 @@
       </c>
       <c r="J235" s="109"/>
     </row>
-    <row r="236" spans="3:10">
+    <row r="236" spans="3:11">
       <c r="C236" s="105" t="s">
         <v>126</v>
       </c>
@@ -6623,7 +6645,7 @@
       </c>
       <c r="J236" s="109"/>
     </row>
-    <row r="239" spans="3:10">
+    <row r="239" spans="3:11">
       <c r="C239" s="102" t="s">
         <v>110</v>
       </c>
@@ -6632,7 +6654,7 @@
       </c>
       <c r="F239" s="104"/>
     </row>
-    <row r="240" spans="3:10">
+    <row r="240" spans="3:11">
       <c r="C240" s="102" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Add our input data for decoder experiments
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4E0D2E-C8C0-3841-A5EB-020618EB5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EF5D1-AE75-F244-B888-CF36E5EA482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -440,9 +440,6 @@
     <t>GPT-4 (decoder)</t>
   </si>
   <si>
-    <t>LLaMA (7B) (decoder)</t>
-  </si>
-  <si>
     <t>Inputs</t>
   </si>
   <si>
@@ -462,6 +459,9 @@
   </si>
   <si>
     <t>Vicuna (13B) (decoder) (zero-shot)</t>
+  </si>
+  <si>
+    <t>Alpaca+LoRA (decoder) (zero-shot)</t>
   </si>
 </sst>
 </file>
@@ -755,7 +755,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1020,8 +1020,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1341,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J215" sqref="J215"/>
+    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="I214" sqref="I214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6337,78 +6335,84 @@
       <c r="I211" s="1"/>
     </row>
     <row r="212" spans="3:9">
-      <c r="C212" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D212" s="110"/>
-      <c r="E212" s="110"/>
-      <c r="F212" s="110"/>
+      <c r="C212" s="112" t="s">
+        <v>139</v>
+      </c>
+      <c r="D212" s="2">
+        <v>0.86839999999999995</v>
+      </c>
+      <c r="E212" s="2">
+        <v>0.85389999999999999</v>
+      </c>
+      <c r="F212" s="2">
+        <v>0.86260000000000003</v>
+      </c>
       <c r="G212" s="2">
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="I212" s="41"/>
     </row>
     <row r="213" spans="3:9">
-      <c r="C213" s="7" t="s">
-        <v>132</v>
+      <c r="C213" s="112" t="s">
+        <v>138</v>
+      </c>
+      <c r="D213" s="8"/>
+      <c r="E213" s="8"/>
+      <c r="F213" s="8"/>
+      <c r="G213" s="2">
+        <v>2048</v>
       </c>
       <c r="I213" s="41"/>
     </row>
     <row r="214" spans="3:9">
       <c r="C214" s="112" t="s">
-        <v>133</v>
-      </c>
-      <c r="D214" s="84"/>
-      <c r="E214" s="84"/>
-      <c r="F214" s="84"/>
+        <v>140</v>
+      </c>
+      <c r="D214" s="8"/>
+      <c r="E214" s="8"/>
+      <c r="F214" s="8"/>
       <c r="G214" s="2">
         <v>2048</v>
       </c>
       <c r="I214" s="41"/>
     </row>
     <row r="215" spans="3:9">
-      <c r="C215" s="112" t="s">
-        <v>140</v>
-      </c>
-      <c r="D215" s="2">
-        <v>0.86839999999999995</v>
-      </c>
-      <c r="E215" s="2">
-        <v>0.85389999999999999</v>
-      </c>
-      <c r="F215" s="2">
-        <v>0.86260000000000003</v>
-      </c>
-      <c r="G215" s="2">
-        <v>2048</v>
+      <c r="C215" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="D215" s="103">
+        <v>0.8468</v>
+      </c>
+      <c r="E215" s="103">
+        <v>0.79490000000000005</v>
+      </c>
+      <c r="F215" s="103">
+        <v>0.84389999999999998</v>
+      </c>
+      <c r="G215" s="89">
+        <v>4096</v>
       </c>
     </row>
     <row r="216" spans="3:9">
-      <c r="C216" s="112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D216" s="8"/>
-      <c r="E216" s="8"/>
-      <c r="F216" s="8"/>
+      <c r="C216" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D216" s="110"/>
+      <c r="E216" s="110"/>
+      <c r="F216" s="110"/>
       <c r="G216" s="2">
-        <v>2048</v>
+        <v>8192</v>
       </c>
     </row>
     <row r="217" spans="3:9">
-      <c r="C217" s="91" t="s">
-        <v>118</v>
-      </c>
-      <c r="D217" s="103">
-        <v>0.8468</v>
-      </c>
-      <c r="E217" s="103">
-        <v>0.79490000000000005</v>
-      </c>
-      <c r="F217" s="103">
-        <v>0.84389999999999998</v>
-      </c>
-      <c r="G217" s="89">
-        <v>4096</v>
+      <c r="C217" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D217" s="8"/>
+      <c r="E217" s="8"/>
+      <c r="F217" s="8"/>
+      <c r="G217" s="2">
+        <v>8192</v>
       </c>
       <c r="I217" s="41"/>
     </row>
@@ -6422,33 +6426,18 @@
       <c r="I220" s="41"/>
     </row>
     <row r="221" spans="3:9">
-      <c r="C221" s="114"/>
-      <c r="D221" s="115"/>
-      <c r="E221" s="115"/>
-      <c r="F221" s="115"/>
-      <c r="G221" s="116"/>
-      <c r="H221" s="116"/>
+      <c r="H221" s="114"/>
       <c r="I221" s="41"/>
     </row>
     <row r="222" spans="3:9">
-      <c r="C222" s="114"/>
-      <c r="D222" s="115"/>
-      <c r="E222" s="115"/>
-      <c r="F222" s="115"/>
-      <c r="G222" s="116"/>
-      <c r="H222" s="116"/>
+      <c r="H222" s="114"/>
     </row>
     <row r="223" spans="3:9">
-      <c r="C223" s="114"/>
-      <c r="D223" s="113"/>
-      <c r="E223" s="113"/>
-      <c r="F223" s="113"/>
-      <c r="G223" s="116"/>
-      <c r="H223" s="116"/>
+      <c r="H223" s="114"/>
     </row>
     <row r="226" spans="3:11">
       <c r="C226" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D226" s="4" t="s">
         <v>0</v>
@@ -6465,7 +6454,7 @@
     </row>
     <row r="227" spans="3:11">
       <c r="C227" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D227" s="4">
         <v>162</v>
@@ -6491,15 +6480,15 @@
     </row>
     <row r="229" spans="3:11">
       <c r="I229" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="K229" t="s">
         <v>136</v>
-      </c>
-      <c r="K229" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="230" spans="3:11">
       <c r="K230" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="234" spans="3:11">

</xml_diff>

<commit_message>
Update results: finetuend Vicuna
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1EF5D1-AE75-F244-B888-CF36E5EA482B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471C5F30-1F3A-E943-8263-6FCD764480B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="142">
   <si>
     <t>MIN</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>Alpaca+LoRA (decoder) (zero-shot)</t>
+  </si>
+  <si>
+    <t>LLaMA (13B) (decoder) (zero-shot)</t>
   </si>
 </sst>
 </file>
@@ -755,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1021,6 +1024,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1339,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="I214" sqref="I214"/>
+    <sheetView tabSelected="1" topLeftCell="B199" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6336,25 +6342,16 @@
     </row>
     <row r="212" spans="3:9">
       <c r="C212" s="112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D212" s="2">
-        <v>0.86839999999999995</v>
-      </c>
-      <c r="E212" s="2">
-        <v>0.85389999999999999</v>
-      </c>
-      <c r="F212" s="2">
-        <v>0.86260000000000003</v>
-      </c>
-      <c r="G212" s="2">
+        <v>141</v>
+      </c>
+      <c r="G212" s="115">
         <v>2048</v>
       </c>
       <c r="I212" s="41"/>
     </row>
     <row r="213" spans="3:9">
       <c r="C213" s="112" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="8"/>
@@ -6366,57 +6363,78 @@
     </row>
     <row r="214" spans="3:9">
       <c r="C214" s="112" t="s">
-        <v>140</v>
-      </c>
-      <c r="D214" s="8"/>
-      <c r="E214" s="8"/>
-      <c r="F214" s="8"/>
+        <v>139</v>
+      </c>
+      <c r="D214" s="2">
+        <v>0.86839999999999995</v>
+      </c>
+      <c r="E214" s="2">
+        <v>0.85389999999999999</v>
+      </c>
+      <c r="F214" s="2">
+        <v>0.86260000000000003</v>
+      </c>
       <c r="G214" s="2">
         <v>2048</v>
       </c>
       <c r="I214" s="41"/>
     </row>
     <row r="215" spans="3:9">
-      <c r="C215" s="91" t="s">
+      <c r="C215" s="112" t="s">
+        <v>138</v>
+      </c>
+      <c r="D215" s="84">
+        <v>0.876</v>
+      </c>
+      <c r="E215" s="84">
+        <v>0.85729999999999995</v>
+      </c>
+      <c r="F215" s="84">
+        <v>0.8679</v>
+      </c>
+      <c r="G215" s="2">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="216" spans="3:9">
+      <c r="C216" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="D215" s="103">
+      <c r="D216" s="103">
         <v>0.8468</v>
       </c>
-      <c r="E215" s="103">
+      <c r="E216" s="103">
         <v>0.79490000000000005</v>
       </c>
-      <c r="F215" s="103">
+      <c r="F216" s="103">
         <v>0.84389999999999998</v>
       </c>
-      <c r="G215" s="89">
+      <c r="G216" s="89">
         <v>4096</v>
-      </c>
-    </row>
-    <row r="216" spans="3:9">
-      <c r="C216" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D216" s="110"/>
-      <c r="E216" s="110"/>
-      <c r="F216" s="110"/>
-      <c r="G216" s="2">
-        <v>8192</v>
       </c>
     </row>
     <row r="217" spans="3:9">
       <c r="C217" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D217" s="8"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
+        <v>130</v>
+      </c>
+      <c r="D217" s="110"/>
+      <c r="E217" s="110"/>
+      <c r="F217" s="110"/>
       <c r="G217" s="2">
         <v>8192</v>
       </c>
       <c r="I217" s="41"/>
     </row>
     <row r="218" spans="3:9">
+      <c r="C218" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D218" s="8"/>
+      <c r="E218" s="8"/>
+      <c r="F218" s="8"/>
+      <c r="G218" s="2">
+        <v>8192</v>
+      </c>
       <c r="I218" s="41"/>
     </row>
     <row r="219" spans="3:9">

</xml_diff>

<commit_message>
Update experiment results for alpaca 13b zeroshot as decoder
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0C9B99-7D53-CB42-BBF2-80F2C33DA20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C003F27-731B-C54D-8D4B-BE87F949250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -461,10 +461,10 @@
     <t>Vicuna (13B) (decoder) (zero-shot)</t>
   </si>
   <si>
-    <t>LLaMA+Alpaca (decoder) (zero-shot)</t>
-  </si>
-  <si>
-    <t>LLaMA+Alpaca (decoder) (fine-tuned)</t>
+    <t>Alpaca (decoder) (zero-shot)</t>
+  </si>
+  <si>
+    <t>Alpaca (decoder) (fine-tuned)</t>
   </si>
 </sst>
 </file>
@@ -1348,8 +1348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
   <dimension ref="A2:AE241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="G220" sqref="G220"/>
+    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H213" sqref="H213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6347,9 +6347,15 @@
       <c r="C212" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="D212" s="8"/>
-      <c r="E212" s="8"/>
-      <c r="F212" s="8"/>
+      <c r="D212" s="2">
+        <v>0.87450000000000006</v>
+      </c>
+      <c r="E212" s="2">
+        <v>0.85589999999999999</v>
+      </c>
+      <c r="F212" s="2">
+        <v>0.86909999999999998</v>
+      </c>
       <c r="G212" s="116">
         <v>2048</v>
       </c>

</xml_diff>

<commit_message>
Update finetuned alpaca and its results
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988F12BB-8F98-B844-B3B8-3474AB94AE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BDD2E0-B0E7-CD4A-9B51-C7862471A558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
@@ -758,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1030,6 +1030,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1349,7 +1352,7 @@
   <dimension ref="A2:AE241"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A200" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C218" sqref="C218"/>
+      <selection activeCell="D217" sqref="D217"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6365,6 +6368,15 @@
       <c r="C213" s="112" t="s">
         <v>139</v>
       </c>
+      <c r="D213" s="117">
+        <v>0.87790000000000001</v>
+      </c>
+      <c r="E213" s="117">
+        <v>0.85840000000000005</v>
+      </c>
+      <c r="F213" s="117">
+        <v>0.87039999999999995</v>
+      </c>
       <c r="G213" s="115">
         <v>2048</v>
       </c>

</xml_diff>

<commit_message>
Update experiments results from gpt-4
</commit_message>
<xml_diff>
--- a/dataset/baseline.xlsx
+++ b/dataset/baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quert/Documents/GitHub/edit_NetKu/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BDD2E0-B0E7-CD4A-9B51-C7862471A558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5F8CF3-E99A-FE4E-83DF-C9A3BC70505D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
+    <workbookView xWindow="31060" yWindow="2700" windowWidth="51200" windowHeight="28300" xr2:uid="{9D12E74E-9F27-3646-89FF-1CB4FA5F7B76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="138">
   <si>
     <t>MIN</t>
   </si>
@@ -419,21 +419,6 @@
     <t>ChatGPT (one-shot) min</t>
   </si>
   <si>
-    <t>GPT-3.5 (zero-shot)</t>
-  </si>
-  <si>
-    <t>GPT-3.5 (one-shot) max</t>
-  </si>
-  <si>
-    <t>GPT-3.5 (one-shot) mean</t>
-  </si>
-  <si>
-    <t>GPT-3.5 (one-shot) min</t>
-  </si>
-  <si>
-    <t>GPT-4 (zero-shot)</t>
-  </si>
-  <si>
     <t>GPT-3.5 (decoder)</t>
   </si>
   <si>
@@ -465,6 +450,9 @@
   </si>
   <si>
     <t>Vicuna-NetKu-13B</t>
+  </si>
+  <si>
+    <t>BART</t>
   </si>
 </sst>
 </file>
@@ -758,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,22 +1005,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1349,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ED6EA46-1DAB-8E45-A9C2-F32EDA5E4B78}">
-  <dimension ref="A2:AE241"/>
+  <dimension ref="A2:AF241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D217" sqref="D217"/>
+    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="M212" sqref="M212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1732,7 +1719,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="2:31">
+    <row r="17" spans="2:32">
       <c r="C17" s="4" t="s">
         <v>22</v>
       </c>
@@ -1748,8 +1735,11 @@
       <c r="G17" s="37">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="2:31">
+      <c r="AB17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="2:32">
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1795,8 +1785,21 @@
       <c r="Z18" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:31">
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF18" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:32">
       <c r="C19" s="13"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
@@ -1832,8 +1835,23 @@
       <c r="Z19" s="37">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="2:31">
+      <c r="AB19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC19" s="4">
+        <v>77</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>86561</v>
+      </c>
+      <c r="AE19" s="80">
+        <v>7775.1786000000002</v>
+      </c>
+      <c r="AF19" s="37">
+        <v>4388.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:32">
       <c r="O20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1864,8 +1882,23 @@
       <c r="Z20" s="37">
         <v>2153</v>
       </c>
-    </row>
-    <row r="21" spans="2:31">
+      <c r="AB20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC20" s="4">
+        <v>27</v>
+      </c>
+      <c r="AD20" s="4">
+        <v>73677</v>
+      </c>
+      <c r="AE20" s="80">
+        <v>6218.1310000000003</v>
+      </c>
+      <c r="AF20" s="37">
+        <v>3511.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:32">
       <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
@@ -1882,7 +1915,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="2:31">
+    <row r="22" spans="2:32">
       <c r="C22" s="18" t="s">
         <v>9</v>
       </c>
@@ -1905,7 +1938,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:31">
+    <row r="23" spans="2:32">
       <c r="B23" s="60"/>
       <c r="C23" s="60"/>
       <c r="D23" s="60"/>
@@ -1926,7 +1959,7 @@
       <c r="S23" s="60"/>
       <c r="T23" s="60"/>
     </row>
-    <row r="24" spans="2:31">
+    <row r="24" spans="2:32">
       <c r="C24" s="38" t="s">
         <v>32</v>
       </c>
@@ -1934,7 +1967,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="2:31">
+    <row r="25" spans="2:32">
       <c r="C25" s="17"/>
       <c r="D25" s="19" t="s">
         <v>26</v>
@@ -1967,7 +2000,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:31">
+    <row r="26" spans="2:32">
       <c r="C26" s="23"/>
       <c r="D26" s="23" t="s">
         <v>0</v>
@@ -2010,7 +2043,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="27" spans="2:31">
+    <row r="27" spans="2:32">
       <c r="C27" s="25" t="s">
         <v>11</v>
       </c>
@@ -2057,7 +2090,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="28" spans="2:31">
+    <row r="28" spans="2:32">
       <c r="C28" s="27" t="s">
         <v>12</v>
       </c>
@@ -2089,7 +2122,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:31">
+    <row r="29" spans="2:32">
       <c r="C29" s="4" t="s">
         <v>22</v>
       </c>
@@ -2121,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:31">
+    <row r="30" spans="2:32">
       <c r="C30" s="4" t="s">
         <v>21</v>
       </c>
@@ -2154,7 +2187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:31">
+    <row r="31" spans="2:32">
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -2167,7 +2200,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="2:31">
+    <row r="32" spans="2:32">
       <c r="C32" s="76" t="s">
         <v>26</v>
       </c>
@@ -6182,15 +6215,13 @@
     </row>
     <row r="202" spans="1:18">
       <c r="B202" s="41"/>
-      <c r="C202" s="111"/>
-      <c r="D202" s="111"/>
-      <c r="E202" s="111"/>
-      <c r="F202" s="111"/>
-      <c r="G202" s="111"/>
-      <c r="H202" s="113"/>
+      <c r="C202" s="110"/>
+      <c r="D202" s="110"/>
+      <c r="E202" s="110"/>
+      <c r="F202" s="110"/>
     </row>
     <row r="203" spans="1:18">
-      <c r="C203" s="111"/>
+      <c r="C203" s="110"/>
       <c r="D203" s="89" t="s">
         <v>14</v>
       </c>
@@ -6200,26 +6231,43 @@
       <c r="F203" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="G203" s="89" t="s">
+      <c r="G203" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="H203" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="I203" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="J203" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="K203" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="L203" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="M203" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H203" s="113"/>
-      <c r="I203" s="1"/>
     </row>
     <row r="204" spans="1:18">
       <c r="C204" s="7" t="s">
         <v>115</v>
       </c>
       <c r="D204" s="84">
-        <v>0.98160000000000003</v>
+        <v>0.98670000000000002</v>
       </c>
       <c r="E204" s="84">
-        <v>0.97489999999999999</v>
-      </c>
-      <c r="F204" s="84">
-        <v>0.98140000000000005</v>
+        <v>0.98309999999999997</v>
+      </c>
+      <c r="F204" s="112">
+        <v>0.98619999999999997</v>
       </c>
       <c r="I204" s="1"/>
+      <c r="L204" s="115"/>
     </row>
     <row r="205" spans="1:18">
       <c r="C205" s="7" t="s">
@@ -6231,13 +6279,30 @@
       <c r="E205" s="84">
         <v>3.7199999999999997E-2</v>
       </c>
-      <c r="F205" s="84">
+      <c r="F205" s="112">
         <v>6.7599999999999993E-2</v>
       </c>
-      <c r="G205" s="2">
+      <c r="G205" s="112">
+        <v>0.8256</v>
+      </c>
+      <c r="H205" s="112">
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="I205" s="112">
+        <v>0.60070000000000001</v>
+      </c>
+      <c r="J205" s="112">
+        <v>0.54110000000000003</v>
+      </c>
+      <c r="K205" s="112">
+        <v>0.61009999999999998</v>
+      </c>
+      <c r="L205" s="117">
+        <v>0.87</v>
+      </c>
+      <c r="M205" s="34">
         <v>4096</v>
       </c>
-      <c r="I205" s="1"/>
     </row>
     <row r="206" spans="1:18">
       <c r="C206" s="7" t="s">
@@ -6252,14 +6317,31 @@
       <c r="F206" s="84">
         <v>0.51790000000000003</v>
       </c>
-      <c r="G206" s="2">
+      <c r="G206" s="112">
+        <v>0.59989999999999999</v>
+      </c>
+      <c r="H206" s="112">
+        <v>0.77849999999999997</v>
+      </c>
+      <c r="I206" s="112">
+        <v>0.78990000000000005</v>
+      </c>
+      <c r="J206" s="112">
+        <v>0.7641</v>
+      </c>
+      <c r="K206" s="112">
+        <v>0.49419999999999997</v>
+      </c>
+      <c r="L206" s="117">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="M206" s="2">
         <v>4096</v>
       </c>
-      <c r="I206" s="1"/>
     </row>
     <row r="207" spans="1:18">
       <c r="C207" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D207" s="84">
         <v>0.88149999999999995</v>
@@ -6270,213 +6352,172 @@
       <c r="F207" s="84">
         <v>0.87780000000000002</v>
       </c>
-      <c r="G207" s="2">
+      <c r="G207" s="113"/>
+      <c r="H207" s="113"/>
+      <c r="I207" s="34"/>
+      <c r="J207" s="113"/>
+      <c r="K207" s="113"/>
+      <c r="L207" s="116"/>
+      <c r="M207" s="2">
         <v>4096</v>
       </c>
-      <c r="I207" s="1"/>
     </row>
     <row r="208" spans="1:18">
-      <c r="C208" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D208" s="84">
-        <v>0.34439999999999998</v>
-      </c>
-      <c r="E208" s="84">
-        <v>0.17019999999999999</v>
-      </c>
-      <c r="F208" s="84">
-        <v>0.32240000000000002</v>
-      </c>
-      <c r="G208" s="2">
-        <v>4096</v>
-      </c>
-      <c r="I208" s="1"/>
-      <c r="P208" s="2"/>
-    </row>
-    <row r="209" spans="3:9">
-      <c r="C209" s="7" t="s">
+      <c r="C208" s="111" t="s">
+        <v>133</v>
+      </c>
+      <c r="D208" s="2">
+        <v>0.87450000000000006</v>
+      </c>
+      <c r="E208" s="2">
+        <v>0.85589999999999999</v>
+      </c>
+      <c r="F208" s="2">
+        <v>0.86909999999999998</v>
+      </c>
+      <c r="G208" s="113"/>
+      <c r="H208" s="113"/>
+      <c r="I208" s="114"/>
+      <c r="J208" s="113"/>
+      <c r="K208" s="113"/>
+      <c r="L208" s="116"/>
+      <c r="M208" s="2">
+        <v>2048</v>
+      </c>
+      <c r="P208" s="1"/>
+    </row>
+    <row r="209" spans="3:13">
+      <c r="C209" s="111" t="s">
+        <v>134</v>
+      </c>
+      <c r="D209" s="47">
+        <v>0.87790000000000001</v>
+      </c>
+      <c r="E209" s="47">
+        <v>0.85840000000000005</v>
+      </c>
+      <c r="F209" s="47">
+        <v>0.87039999999999995</v>
+      </c>
+      <c r="G209" s="113"/>
+      <c r="H209" s="113"/>
+      <c r="I209" s="114"/>
+      <c r="J209" s="113"/>
+      <c r="K209" s="113"/>
+      <c r="L209" s="116"/>
+      <c r="M209" s="1">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="210" spans="3:13">
+      <c r="C210" s="111" t="s">
+        <v>135</v>
+      </c>
+      <c r="D210" s="2">
+        <v>0.86839999999999995</v>
+      </c>
+      <c r="E210" s="2">
+        <v>0.85389999999999999</v>
+      </c>
+      <c r="F210" s="2">
+        <v>0.86260000000000003</v>
+      </c>
+      <c r="G210" s="113"/>
+      <c r="H210" s="113"/>
+      <c r="I210" s="114"/>
+      <c r="J210" s="113"/>
+      <c r="K210" s="113"/>
+      <c r="L210" s="116"/>
+      <c r="M210" s="2">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="211" spans="3:13">
+      <c r="C211" s="111" t="s">
+        <v>136</v>
+      </c>
+      <c r="D211" s="84">
+        <v>0.876</v>
+      </c>
+      <c r="E211" s="84">
+        <v>0.85729999999999995</v>
+      </c>
+      <c r="F211" s="84">
+        <v>0.8679</v>
+      </c>
+      <c r="G211" s="113"/>
+      <c r="H211" s="113"/>
+      <c r="I211" s="113"/>
+      <c r="J211" s="113"/>
+      <c r="K211" s="113"/>
+      <c r="L211" s="116"/>
+      <c r="M211" s="2">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="212" spans="3:13">
+      <c r="C212" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D209" s="84">
-        <v>0.42970000000000003</v>
-      </c>
-      <c r="E209" s="84">
-        <v>0.2427</v>
-      </c>
-      <c r="F209" s="84">
-        <v>0.40739999999999998</v>
-      </c>
-      <c r="G209" s="2">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="210" spans="3:9">
-      <c r="C210" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D210" s="84">
-        <v>0.44040000000000001</v>
-      </c>
-      <c r="E210" s="84">
-        <v>0.24729999999999999</v>
-      </c>
-      <c r="F210" s="84">
-        <v>0.41170000000000001</v>
-      </c>
-      <c r="G210" s="2">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="211" spans="3:9">
-      <c r="C211" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="D211" s="84">
-        <v>0.44700000000000001</v>
-      </c>
-      <c r="E211" s="84">
-        <v>0.25440000000000002</v>
-      </c>
-      <c r="F211" s="84">
-        <v>0.42159999999999997</v>
-      </c>
-      <c r="G211" s="2">
-        <v>4096</v>
-      </c>
-      <c r="I211" s="1"/>
-    </row>
-    <row r="212" spans="3:9">
-      <c r="C212" s="112" t="s">
-        <v>138</v>
-      </c>
-      <c r="D212" s="2">
-        <v>0.87450000000000006</v>
+      <c r="D212" s="84">
+        <v>0.87360000000000004</v>
       </c>
       <c r="E212" s="2">
-        <v>0.85589999999999999</v>
+        <v>0.85519999999999996</v>
       </c>
       <c r="F212" s="2">
-        <v>0.86909999999999998</v>
-      </c>
-      <c r="G212" s="116">
-        <v>2048</v>
-      </c>
-      <c r="I212" s="41"/>
-    </row>
-    <row r="213" spans="3:9">
-      <c r="C213" s="112" t="s">
-        <v>139</v>
-      </c>
-      <c r="D213" s="117">
-        <v>0.87790000000000001</v>
-      </c>
-      <c r="E213" s="117">
-        <v>0.85840000000000005</v>
-      </c>
-      <c r="F213" s="117">
-        <v>0.87039999999999995</v>
-      </c>
-      <c r="G213" s="115">
-        <v>2048</v>
-      </c>
-      <c r="I213" s="41"/>
-    </row>
-    <row r="214" spans="3:9">
-      <c r="C214" s="112" t="s">
-        <v>140</v>
-      </c>
-      <c r="D214" s="2">
-        <v>0.86839999999999995</v>
-      </c>
-      <c r="E214" s="2">
-        <v>0.85389999999999999</v>
-      </c>
-      <c r="F214" s="2">
-        <v>0.86260000000000003</v>
-      </c>
-      <c r="G214" s="2">
-        <v>2048</v>
-      </c>
-      <c r="I214" s="41"/>
-    </row>
-    <row r="215" spans="3:9">
-      <c r="C215" s="112" t="s">
-        <v>141</v>
-      </c>
-      <c r="D215" s="84">
-        <v>0.876</v>
-      </c>
-      <c r="E215" s="84">
-        <v>0.85729999999999995</v>
-      </c>
-      <c r="F215" s="84">
-        <v>0.8679</v>
-      </c>
-      <c r="G215" s="2">
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="216" spans="3:9">
-      <c r="C216" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D216" s="110"/>
-      <c r="E216" s="110"/>
-      <c r="F216" s="110"/>
-      <c r="G216" s="2">
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="217" spans="3:9">
-      <c r="C217" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D217" s="110"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="G217" s="2">
-        <v>4096</v>
-      </c>
-      <c r="I217" s="41"/>
-    </row>
-    <row r="218" spans="3:9">
-      <c r="C218" s="91" t="s">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="G212" s="8"/>
+      <c r="H212" s="8"/>
+      <c r="I212" s="7"/>
+      <c r="J212" s="8"/>
+      <c r="K212" s="8"/>
+      <c r="L212" s="118">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="M212" s="2"/>
+    </row>
+    <row r="213" spans="3:13">
+      <c r="C213" s="91" t="s">
         <v>118</v>
       </c>
-      <c r="D218" s="103">
+      <c r="D213" s="103">
         <v>0.8468</v>
       </c>
-      <c r="E218" s="103">
+      <c r="E213" s="103">
         <v>0.79490000000000005</v>
       </c>
-      <c r="F218" s="103">
+      <c r="F213" s="103">
         <v>0.84389999999999998</v>
       </c>
-      <c r="G218" s="89">
-        <v>4096</v>
-      </c>
-      <c r="I218" s="41"/>
-    </row>
-    <row r="219" spans="3:9">
+      <c r="G213" s="8"/>
+      <c r="H213" s="8"/>
+      <c r="I213" s="8"/>
+      <c r="J213" s="8"/>
+      <c r="K213" s="8"/>
+      <c r="L213" s="8"/>
+      <c r="M213" s="8"/>
+    </row>
+    <row r="219" spans="3:13">
       <c r="I219" s="41"/>
     </row>
-    <row r="220" spans="3:9">
+    <row r="220" spans="3:13">
       <c r="I220" s="41"/>
     </row>
-    <row r="221" spans="3:9">
-      <c r="H221" s="114"/>
+    <row r="221" spans="3:13">
+      <c r="H221" s="1"/>
       <c r="I221" s="41"/>
     </row>
-    <row r="222" spans="3:9">
-      <c r="H222" s="114"/>
-    </row>
-    <row r="223" spans="3:9">
-      <c r="H223" s="114"/>
+    <row r="222" spans="3:13">
+      <c r="H222" s="1"/>
+    </row>
+    <row r="223" spans="3:13">
+      <c r="H223" s="1"/>
     </row>
     <row r="226" spans="3:11">
       <c r="C226" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D226" s="4" t="s">
         <v>0</v>
@@ -6493,7 +6534,7 @@
     </row>
     <row r="227" spans="3:11">
       <c r="C227" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D227" s="4">
         <v>162</v>
@@ -6519,15 +6560,15 @@
     </row>
     <row r="229" spans="3:11">
       <c r="I229" s="15" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K229" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="230" spans="3:11">
       <c r="K230" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="234" spans="3:11">

</xml_diff>